<commit_message>
feat: ambito 1 prompts completos
</commit_message>
<xml_diff>
--- a/resultados/06/comparacion_puntajes.xlsx
+++ b/resultados/06/comparacion_puntajes.xlsx
@@ -426,13 +426,13 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E2">
         <v>4</v>
@@ -449,13 +449,13 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C3">
         <v>4</v>
       </c>
       <c r="D3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E3">
         <v>4</v>
@@ -464,7 +464,7 @@
         <v>2</v>
       </c>
       <c r="G3">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -472,19 +472,19 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C4">
         <v>4</v>
       </c>
       <c r="D4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E4">
         <v>4</v>
       </c>
       <c r="F4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G4">
         <v>3</v>
@@ -495,13 +495,13 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C5">
         <v>4</v>
       </c>
       <c r="D5">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E5">
         <v>4</v>
@@ -510,7 +510,7 @@
         <v>3</v>
       </c>
       <c r="G5">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -518,22 +518,22 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E6">
         <v>4</v>
       </c>
       <c r="F6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G6">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -541,19 +541,19 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C7">
         <v>4</v>
       </c>
       <c r="D7">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E7">
         <v>3</v>
       </c>
       <c r="F7">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G7">
         <v>4</v>
@@ -564,22 +564,22 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C8">
         <v>4</v>
       </c>
       <c r="D8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E8">
         <v>4</v>
       </c>
       <c r="F8">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G8">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -587,13 +587,13 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C9">
         <v>4</v>
       </c>
       <c r="D9">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E9">
         <v>4</v>
@@ -610,19 +610,19 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C10">
         <v>4</v>
       </c>
       <c r="D10">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E10">
         <v>4</v>
       </c>
       <c r="F10">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G10">
         <v>3</v>
@@ -633,22 +633,22 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C11">
         <v>4</v>
       </c>
       <c r="D11">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E11">
         <v>4</v>
       </c>
       <c r="F11">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G11">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -656,19 +656,19 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C12">
         <v>4</v>
       </c>
       <c r="D12">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E12">
         <v>4</v>
       </c>
       <c r="F12">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G12">
         <v>3</v>
@@ -679,19 +679,19 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C13">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D13">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E13">
         <v>4</v>
       </c>
       <c r="F13">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G13">
         <v>2</v>
@@ -702,16 +702,16 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C14">
         <v>4</v>
       </c>
       <c r="D14">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E14">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F14">
         <v>2</v>
@@ -725,7 +725,7 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C15">
         <v>4</v>
@@ -740,7 +740,7 @@
         <v>1</v>
       </c>
       <c r="G15">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -748,7 +748,7 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C16">
         <v>4</v>
@@ -757,13 +757,13 @@
         <v>2</v>
       </c>
       <c r="E16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F16">
         <v>2</v>
       </c>
       <c r="G16">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -771,22 +771,22 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C17">
         <v>4</v>
       </c>
       <c r="D17">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E17">
         <v>4</v>
       </c>
       <c r="F17">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G17">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -794,19 +794,19 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C18">
         <v>4</v>
       </c>
       <c r="D18">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E18">
         <v>4</v>
       </c>
       <c r="F18">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G18">
         <v>2</v>
@@ -817,19 +817,19 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C19">
         <v>4</v>
       </c>
       <c r="D19">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E19">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F19">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G19">
         <v>3</v>
@@ -840,19 +840,19 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C20">
         <v>4</v>
       </c>
       <c r="D20">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E20">
         <v>4</v>
       </c>
       <c r="F20">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G20">
         <v>1</v>
@@ -863,13 +863,13 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C21">
         <v>4</v>
       </c>
       <c r="D21">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E21">
         <v>4</v>
@@ -878,7 +878,7 @@
         <v>3</v>
       </c>
       <c r="G21">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: enfoque07 de referencias para ámbito 1 de escritura
</commit_message>
<xml_diff>
--- a/resultados/06/comparacion_puntajes.xlsx
+++ b/resultados/06/comparacion_puntajes.xlsx
@@ -482,30 +482,30 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C2" s="2" t="n">
         <v>2</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="n"/>
       <c r="B3" s="2" t="inlineStr">
         <is>
-          <t>Aparece el tema general (pandemia y la “realidad del trabajo permanente”) y hay una alusión temporal vaga («nuestra actual pandemia»), pero faltan elementos esenciales: no se nombran actores concretos (solo referencias genéricas a empleados/empleadores), no se especifica un lugar/contexto espacial claro (se habla de casa o barrios de manera imprecisa) y la presentación inicial es confusa y dispersa. Además la introducción no articula claramente el problema del reactivo (la idea del hogar como último refugio en riesgo) ni plantea con precisión la pregunta que guiaría el texto. Sugerencia: redactar 1–2 oraciones precisas que indiquen qué se examina, quiénes son los actores relevantes (ej. trabajadores remotos, empleadores, autoridades sanitarias), dónde (hogares/ambiente doméstico a nivel nacional/internacional) y cuándo (pandemia de COVID‑19, años 2020–2021).</t>
+          <t>El texto inicia con una referencia temporal clara («nuestra actual pandemia») y plantea un tema general (salud mental y trabajo permanente), pero falla en los otros elementos exigidos: no identifica actores específicos en la introducción (solo aparece vagamente 'sus propios asociados' y más tarde 'empleados/empleadores'), no señala un lugar o contexto espacial preciso (no hay referencia al 'hogar' como espacio-refugio en la introducción) y el tema está formulado de manera imprecisa. En relación al reactivo, la introducción no sitúa explícitamente la tensión central (la vulneración del hogar como refugio) ni presenta con claridad quiénes y dónde serían afectados.</t>
         </is>
       </c>
       <c r="C3" s="2" t="inlineStr">
         <is>
-          <t>Hay un intento de cierre en el último párrafo («El trabajo remoto necesita ser estructurado...» y propuestas breves), pero no cumple con una síntesis clara ni con una proyección articulada: no reformula la idea central en términos nuevos ni extrae implicaciones o recomendaciones desarrolladas; las propuestas finales son vagas y el texto termina abruptamente. No se cierra el argumento sobre el hogar como refugio ni se indican consecuencias concretas o pasos futuros. Sugerencia: elaborar una conclusión que reformule la tesis central y presente implicaciones políticas y sociales concretas (regulación, protección del hogar, medidas prácticas) y una frase final que proyecte futuras líneas de acción o investigación.</t>
+          <t>El cierre ofrece recomendaciones concretas (estructurar el trabajo remoto, uso de cybercafés, bloqueo de llamadas) y por tanto presenta una proyección/práctica, pero carece de una síntesis clara: no reformula la idea principal en palabras nuevas ni integra los argumentos previos en un cierre coherente. La conclusión es más una lista de soluciones sueltas que una reflexión final sobre las implicaciones. Además no articula de forma contundente las consecuencias para el 'hogar' como último refugio, aspecto central del reactivo.</t>
         </is>
       </c>
       <c r="D3" s="2" t="inlineStr">
         <is>
-          <t>La progresión muestra párrafos con temas relacionados pero parcial redundancia: el segundo párrafo (regulación/explotación) y el cuarto (comodidad/flexibilidad mal entendida) repiten tesis similares sobre la explotación del trabajador remoto; además faltan conectores lógicos consistentes y las transiciones son abruptas. Algunas ideas (p. ej. la noción del hogar como refugio en riesgo, núcleo del reactivo) no se desarrollan de forma específica y quedan dispersas entre párrafos. La estructura podría mejorar asignando a cada párrafo un subtema único (historia/contexto, regulación y derechos, efectos psicológicos en el hogar, desmitificación de la flexibilidad, propuestas) y usando conectores claros; también corregir problemas de coherencia y redundancia léxica.</t>
+          <t>El texto está dividido en párrafos que intentan abordar subtemas distintos (introducción, regulación y explotación, efectos psicológicos, crítica a la 'comodidad', propuestas), pero hay repetición temática notable: el cuarto párrafo retoma y repite parcialmente la crítica a la comodidad/flexibilidad ya presente en párrafos anteriores; varias ideas vuelven a formularse sin aportar desarrollo nuevo. Además faltan conectores lógicos consistentes y las transiciones son pobres, lo que dificulta la coherencia global y la lectura. En consecuencia hay redundancia parcial (puntaje 2) y el tratamiento del aspecto central del reactivo (el hogar como refugio) no se desarrolla de forma sistemática en distintos párrafos.</t>
         </is>
       </c>
     </row>
@@ -515,27 +515,27 @@
         <v>2</v>
       </c>
       <c r="C4" s="2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="n"/>
       <c r="B5" s="2" t="inlineStr">
         <is>
-          <t>Solo 1-2 elementos son identificables y de forma vaga. Qué: hay un tema reconocible (salud mental y teletrabajo/hogar) pero no está definido de manera clara y concisa en 1-2 oraciones ni se formula una tesis precisa. Quiénes: aparecen grupos genéricos (empleados, empleadores, trabajadores) pero no se especifican actores concretos ni se delimitan por nombre, sector o característica poblacional. Dónde: prácticamente ausente; solo hay una mención tangencial a 'Japón' al final que no fija el contexto espacial de la introducción. Cuándo: referencias temporales vagas ('nuestra actual pandemia', 'últimos treinta años', 'poco más de cien años') sin precisar el periodo COVID-19 (años) ni acotar el marco temporal del estudio. Respecto al reactivo, el texto alude al problema planteado (pandemia y teletrabajo que pone en peligro el hogar) pero lo hace de forma difusa y discursiva, sin cumplir los requisitos exigidos de especificidad espacial, temporal y de actores. Por ello, y aplicando estrictamente la escala, corresponde NIVEL 2.</t>
+          <t>Se identifican elementos pero varios son vagos o están fuera de foco. Qué: hay un tema general (salud mental y la “realidad del trabajo permanente”) pero la formulación es confusa, no aparece definido de forma clara en 1–2 oraciones y no se centra explícitamente en el teletrabajo y el hogar. Quiénes: solo aparecen referencias genéricas ('empleados', 'empleadores', 'trabajadores'); no hay actores concretos por nombre, sector o institución. Dónde: falta una ubicación geográfica o contexto espacial específico dentro de la introducción (la mención a 'Japón' aparece en un párrafo posterior y no contextualiza la introducción). Cuándo: se alude a la 'actual pandemia' pero no se especifica COVID-19 ni un periodo temporal preciso. En conjunto, el texto no responde con la precisión exigida por el reactivo (teletrabajo y la noción del hogar durante la pandemia) y la redacción impide claridad y especificidad.</t>
         </is>
       </c>
       <c r="C5" s="2" t="inlineStr">
         <is>
-          <t>Hay un cierre reconocible en forma de comentario y recomendaciones (necesidad de estructurar el trabajo remoto; propuestas como cybercafés y bloqueo de llamadas), por eso no puede ser nivel 1 o 2. Sin embargo, falta una síntesis clara: la conclusión no reformula en nuevas palabras la idea principal del texto (que el hogar como refugio frente al trabajo permanente está en riesgo). La proyección existe pero es limitada y práctica (medidas puntuales) y no desarrolla consecuencias más amplias ni conecta explícitamente con el reactivo (p. ej. implicaciones para la salud del hogar, políticas públicas o cambios sociales futuros). Para mejorar: añadir 1–2 oraciones que reexpresen la tesis central sobre el peligro para el hogar y ampliar la proyección hacia consecuencias y posibles políticas o reflexiones futuras.</t>
+          <t>El texto termina con una propuesta (estructurar el teletrabajo, usar cybercafés, bloqueo de llamadas) que constituye proyección, pero carece de una síntesis clara: no reformula en nuevas palabras la idea central sobre el hogar como último refugio amenazado por el trabajo permanente ni relaciona explícitamente las soluciones con esa tesis. La proyección es breve y poco desarrollada, además de redactada con errores y conexiones débiles, por lo que funciona más como un comentario final que como un cierre concluyente.</t>
         </is>
       </c>
       <c r="D5" s="2" t="inlineStr">
         <is>
-          <t>Se identifican cinco párrafos claramente distinguibles, pero existe repetición de ideas en al menos un párrafo, por lo que no alcanza el nivel máximo. Específicamente, el párrafo 4 (“Se comenta mucho...estas bajo contrato.”) recicla la misma tesis principal ya tratada en los párrafos 2 y 3 (que la flexibilidad/comodidad del teletrabajo es en realidad una imposición y fuente de perjuicio), por lo que hay solapamiento temático. Los párrafos 2 y 3, en cambio, desarrollan subtemas distintos y pertinentes (2 = déficit de regulación/explotación; 3 = efectos psicológicos sobre sueño y rutinas). Además, faltan conectores lógicos claros entre párrafos: las transiciones son débiles o inexistentes, lo que dificulta la progresión argumental. En cuanto a pertinencia respecto al reactivo, el texto aborda el peligro para la salud mental y la pérdida del hogar como refugio, pero contiene digresiones (ej. la referencia histórica tangencial en el primer párrafo) que merman la coherencia. Para alcanzar nivel 4 bastaría que el párrafo 4 se reformule para aportar un subtema nuevo (por ejemplo: evidencia empírica, datos estadísticos o propuestas institucionales claras) y que se añadan conectores transicionales breves al inicio de cada párrafo (p. ej. “Además”, “Por ello”, “En contraste”, “En consecuencia”).</t>
+          <t>Los párrafos son identificables y la mayoría presenta subtemas distintos (1: introducción y pregunta; 2: regulación y riesgo de explotación; 3: efectos sobre rutinas y salud mental; 5: propuestas). Sin embargo, el párrafo 4 repite ideas ya expuestas en el párrafo 2 (imposición del empleador, falsa comodidad/flexibilidad y explotación), por lo que existe repetición de información en un párrafo. Además faltan conectores lógicos claros entre párrafos (no hay transiciones que articulen la progresión de la introducción a la exposición de riesgos, al impacto psicológico y a las propuestas), y el texto no atiende con suficiente precisión el aspecto central del reactivo —la idea del hogar como último refugio cuya salud se ve amenazada—; ese eje queda implícito pero no desarrollado. Por estas deficiencias (una repetición explícita y ausencia de conectores y de foco en el reactivo) corresponde puntuar 2.</t>
         </is>
       </c>
     </row>
@@ -544,60 +544,60 @@
         <v>2</v>
       </c>
       <c r="B6" s="2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C6" s="2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D6" s="2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="n"/>
       <c r="B7" s="2" t="inlineStr">
         <is>
-          <t>Presenta el 'qué' (pandemia y aprendizaje virtual) y el 'quién' (niños y adolescentes) y menciona un ámbito general ('en todo el mundo'), pero falla en la especificidad requerida: el 'dónde' es demasiado genérico y el 'cuándo' queda implícito en ‘la pandemia’ sin fechas o periodo claro. Para alcanzar nivel 4 se requiere precisar el contexto espacial (país, región o tipo de sistema educativo) y acotar temporalmente (fecha, año o fase de la pandemia), además de identificar actores concretos relevantes (por ejemplo: estudiantes, docentes, autoridades educativas, familias).</t>
+          <t>El texto presenta el tema central (impacto de la pandemia en el aprendizaje) y el ámbito espacial general ('en todo el mundo') y menciona el grupo afectado ('niños y adolescentes'), pero falla en especificidad temporal y en precisión de actores: 'pandemia' no aporta un marco cronológico concreto (fechas o periodo) y no se nombran actores institucionales relevantes (escuelas, autoridades educativas, familias como sujeto activo). Además la apertura termina en una pregunta abrupta y no establece con claridad el enfoque del reactivo (posturas sobre presencialidad vs virtualidad).</t>
         </is>
       </c>
       <c r="C7" s="2" t="inlineStr">
         <is>
-          <t>El cierre final contiene proyecciones y recomendaciones (evitar interacción hasta inmunidad de rebaño; responsabilidad familiar para incentivar protocolos), pero no ofrece una síntesis clara que reformule la idea principal con otras palabras. La proyección existe pero es débil y parcialmente justificada; falta una oración que recapitule la tesis sobre el impacto del aprendizaje virtual y vincule explícitamente las recomendaciones con las evidencias presentadas. Para nivel 4 se necesita una reformulación concisa de la conclusión y una proyección más explícita y argumentada.</t>
+          <t>Existe un intento de cierre en los últimos párrafos (se sugieren medidas sanitarias y que el núcleo familiar incentive protocolos), lo cual constituye una proyección práctica, pero falta una síntesis clara y reformulación de la idea principal en palabras nuevas. El cierre ofrece recomendaciones puntuales pero no resume ni evalúa el argumento central ni contrapone las posiciones del reactivo (quedarse en casa vs reabrir por salud mental), por lo que la función de síntesis está ausente o insuficiente.</t>
         </is>
       </c>
       <c r="D7" s="2" t="inlineStr">
         <is>
-          <t>La organización presenta redundancias y saltos temáticos. Párrafos 4 y 5 repiten la misma idea sobre la primacía de la dinámica familiar frente a la interacción con pares (mismas afirmaciones y citas reiteradas). Párrafos 6 y 7 vuelven a tratar medidas sanitarias y recomendaciones familiares con solapamiento de contenido. Además faltan transiciones claras y oraciones temáticas que marquen subtemas distintos; en varios momentos el texto cambia de enfoque sin puente lógico. Para mejorar: consolidar información repetida, asignar a cada párrafo un subtema único con oración temática clara y añadir conectores que relacionen evidencia, interpretación y recomendación.</t>
+          <t>El texto tiene párrafos con subtemas identificables, pero presenta redundancias y mala conexión entre ellos: el segundo y tercero repiten la clasificación de áreas de aprendizaje; los párrafos cuarto y quinto reiteran la importancia del entorno familiar y social con solapamientos y citas sin integración crítica. Faltan conectores lógicos consistentes que articulen la transición entre antecedentes, evidencia y recomendaciones. Además no responde de forma balanceada al reactivo (las posturas a favor de mantener la virtualidad o de reabrir por salud mental no se confrontan ni se valoran).</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="n"/>
       <c r="B8" s="2" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C8" s="2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D8" s="2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="n"/>
       <c r="B9" s="2" t="inlineStr">
         <is>
-          <t>Qué: presente y claro (impacto de la pandemia y el aprendizaje virtual en niños y adolescentes), por lo que responde al reactivo. Quiénes: se mencionan “niños y adolescentes” pero de manera genérica; faltan actores concretos (ej.: estudiantes de educación primaria/ secundaria, docentes, padres o autoridades educativas por nombre o categoría). Dónde: demasiado general (“en todo el mundo”); no se especifica país, región o contexto escolar que delimite el análisis. Cuándo: ausente como periodo preciso; solo se alude a la pandemia sin indicar fechas o intervalo (p. ej. 2020–2021). Para alcanzar NIVEL 4 se debe añadir de forma mínima y realista: (1) el periodo temporal exacto al que se refiere la investigación (fechas o años), (2) la ubicación geográfica o contexto institucional concreto (país, región o tipo de colegio), y (3) precisar los actores implicados (tipo de estudiantes y otros agentes relevantes).</t>
+          <t>Presenta el Qué (impacto del aprendizaje virtual en niños y adolescentes, formulado como pregunta) y el Quiénes (niños y adolescentes). Sin embargo, falla en Dónde (solo dice “en todo el mundo”, que es demasiado general; no se especifica país, región o contexto escolar concreto) y en Cuándo (no hay periodo o fechas precisas: no se indica, por ejemplo, 2020–2021 o el inicio de la pandemia). Además, no menciona explícitamente el cierre de colegios ni los actores concretos relevantes al reactivo (autoridades educativas, familias, docentes) ni las posturas enfrentadas sobre la presencialidad, por lo que la introducción no responde plenamente al reactivo. Para alcanzar 3 puntos bastaría con agregar en 1–2 oraciones la ubicación específica (país o región), un periodo concreto (p. ej. desde 2020) y una referencia explícita a los cierres escolares y a los actores/posiciones enfrentadas.</t>
         </is>
       </c>
       <c r="C9" s="2" t="inlineStr">
         <is>
-          <t>El cierre ofrece una proyección (recomienda evitar la interacción hasta alcanzar inmunidad colectiva y pide que la familia incorpore protocolos), por lo que hay comentario final. Sin embargo carece de una síntesis clara que reformule la idea central del texto en nuevas palabras; tampoco responde de manera explícita y equilibrada al reactivo (no valora suficientemente el dilema presencialidad vs salud mental ni ofrece consecuencias o tiempos claros). En resumen: hay proyección parcial pero falla la síntesis y la resolución explícita del problema planteado.</t>
+          <t>La última oración constituye una proyección práctica (recomienda que las familias incentiven protocolos para permitir interacciones más seguras), pero carece de síntesis: no reformula en nuevas palabras la idea principal del texto ni ofrece una conclusión clara respecto al reactivo (si conviene mantener la enseñanza virtual o volver a la presencialidad). Es, en esencia, un comentario final y no un cierre que integre y resuelva la tesis; por ello corresponde 2 puntos.</t>
         </is>
       </c>
       <c r="D9" s="2" t="inlineStr">
         <is>
-          <t>Los párrafos son identificables y hay conectores lógicos entre ellos, además el texto responde al reactivo (discute efectos del aprendizaje virtual, la dimensión familiar/social y el riesgo sanitario). Sin embargo, existe repetición de ideas: los párrafos 4 y 5 abordan esencialmente el mismo subtema (la influencia de la dinámica familiar y social en el aprendizaje y sus consecuencias) sin aportar información claramente distinta, lo que constituye una repetición de contenido. El resto de los párrafos presenta subtemas distintos (introducción y pregunta, clasificación de áreas de aprendizaje, interacción entre áreas y estadísticas, riesgo sanitario y medidas, y recomendación familiar) y están conectados, por lo que corresponde NIVEL 3.</t>
+          <t>Hay párrafos claramente identificables, pero se repite información en al menos un párrafo: el párrafo 5 reitera esencialmente lo expuesto en el párrafo 4 (ambos insisten en que la dinámica familiar afecta el aprendizaje y las relaciones sociales, y el segundo solo añade una cita que no aporta un subtema nuevo). Además, la transición entre el párrafo 2 (definición de las cuatro áreas de aprendizaje) y el párrafo 3 (su combinación e impacto) carece de un conector lógico explícito que oriente la progresión; aunque existen conectores en otros saltos, la cohesión es desigual. Finalmente, el texto no responde de forma clara y directa al reactivo: no ofrece una conclusión explícita sobre si deben reabrirse las escuelas o mantenerse virtuales (se limita a señalar riesgos sanitarios y a recomendar medidas familiares), lo que reduce la pertinencia. Por estas razones, y aplicando la escala indicada, corresponde 2 puntos.</t>
         </is>
       </c>
     </row>
@@ -612,34 +612,34 @@
         <v>3</v>
       </c>
       <c r="D10" s="2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="n"/>
       <c r="B11" s="2" t="inlineStr">
         <is>
-          <t>El texto presenta el 'qué' de forma general (actividad física y contaminación) y menciona el tiempo de forma vaga ('a lo largo de la historia', 'actualmente'), pero falla en identificar actores concretos y el lugar: no menciona a los especialistas en medicina citados en el reactivo ni identifica con precisión quiénes (gobierno, ciudadanos, sectores industriales) y dónde sucede el problema (las 'grandes ciudades' sólo aparecen fuera de la introducción). En suma hay 1–2 elementos claros y el reactivo no se integra en la presentación.</t>
+          <t>El texto sí identifica el tema central (actividad física y contaminación) y menciona un actor genérico (el ser humano) y el lugar general (grandes ciudades), pero falla en especificidad y en atender el reactivo: no menciona a los especialistas que emiten la afirmación ni sitúa temporalmente el problema de forma concreta (‘‘A lo largo de la historia’’ es vago). Además el actor relevante propuesto en la tesis (el gobierno) aparece solo al final y no queda integrado como parte clara de la introducción. En conjunto faltan especificidad en ‘quiénes’ (debería nombrar actores clave) y en ‘cuándo’ para alcanzar una introducción completa.</t>
         </is>
       </c>
       <c r="C11" s="2" t="inlineStr">
         <is>
-          <t>Hay una síntesis: se reitera que las medidas gubernamentales provocarían un cambio de actitud y beneficios ambientales y sanitarios. Sin embargo la proyección es genérica y poco desarrollada (no se indican consecuencias concretas, plazos, implicaciones políticas ni cómo se relacionan esas medidas con la limitación del autocuidado señalada en el reactivo). Falta una proyección explícita y fundamentada.</t>
+          <t>La conclusión resume la tesis principal (que medidas gubernamentales inducirán cambios de actitud y reducirán la contaminación) y plantea una proyección sobre efectos positivos para el medio ambiente y la salud. Sin embargo, es un cierre débilmente argumentado y algo repetitivo: aunque cumple ambas funciones (síntesis y proyección), no aborda limitaciones ni evidencia concreta y no confronta con rigor la idea del reactivo sobre la ineficacia de medidas individuales.</t>
         </is>
       </c>
       <c r="D11" s="2" t="inlineStr">
         <is>
-          <t>Los párrafos están separados y proponen medidas distintas, pero hay redundancia: el párrafo sobre incentivos al transporte público y el que refuta la objeción sobre el comportamiento individual repiten la misma afirmación sobre cambio de conducta; además el tercer párrafo (sobre estudios y mascarillas) retoma el mismo objetivo sin un desarrollo diferencial sólido. Faltan conectores lógicos claros y algunas ideas están mal articuladas; se requiere que cada párrafo desarrolle un subtema único y que el texto contraste explícitamente la eficacia del autocuidado frente a medidas estructurales, como exige el reactivo.</t>
+          <t>El texto tiene párrafos con subtemas (incentivar transporte público, campañas contra el tabaquismo/mascarillas, refutación de escepticismo), pero hay repetición parcial de ideas: la apelación al efecto acumulativo del comportamiento individual aparece tanto en el segundo párrafo como en la refutación posterior, y varias propuestas gubernamentales se repiten sin desarrollo nuevo. Los conectores son básicos pero presentes; falta mayor diferenciación y transición argumental entre párrafos y evidencia que aporte avance real entre ellos.</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="n"/>
       <c r="B12" s="2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C12" s="2" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D12" s="2" t="n">
         <v>2</v>
@@ -649,17 +649,17 @@
       <c r="A13" s="2" t="n"/>
       <c r="B13" s="2" t="inlineStr">
         <is>
-          <t>Solo se identifican claramente 1-2 elementos. Qué: aparece (tema general: relación entre actividad física, contaminación y la necesidad de medidas gubernamentales) pero está difuso por una apertura histórica innecesaria y no se reduce a 1-2 oraciones específicas. Quiénes: se mencionan actores genéricos («el gobierno», «las personas»), pero no actores concretos por nombre ni nivel (p. ej., gobierno municipal, gobierno federal, autoridades sanitarias); esto es vago. Dónde: hay una referencia vaga al contexto («las grandes ciudades») pero falta una ubicación geográfica específica (ciudad, región o país). Cuándo: ausente (no hay periodo temporal ni fecha precisa). Además, la introducción no incorpora la referencia clave del reactivo: la postura de los especialistas en medicina sobre que las medidas individuales no modifican las condiciones que generan la contaminación. Para alcanzar NIVEL 4, la introducción debe (brevemente) 1) definir el tema en 1–2 oraciones claras y centradas, 2) nombrar actores concretos (por ejemplo: ‘gobierno municipal de [ciudad]’ o ‘gobierno federal de [país]’ y/o ‘especialistas en medicina’), 3) precisar la ubicación (ciudad/país) y 4) indicar el periodo (p. ej. ‘en la actualidad (2020–2025)’).</t>
+          <t>Solo cumple de forma clara y parcial el 'Qué' (actividad física, contaminación y una tesis sobre medidas gubernamentales), pero no de modo conciso en 1–2 oraciones específicas. Faltan o son vagas las demás exigencias: 'Quiénes' aparece de forma genérica ("el gobierno", "las personas") y no menciona a los actores concretos requeridos por el reactivo (p. ej. "especialistas en medicina"), por lo que no es específico; 'Dónde' no se especifica en la introducción (aunque el cuerpo alude a "grandes ciudades", la primera sección no lo aclara como contexto introductorio); 'Cuándo' es ambiguo ('A lo largo de la historia', 'Actualmente' son marcadores temporales generales, no un periodo preciso). Para alcanzar 3 puntos haga una corrección mínima: sustituir o añadir 1–2 oraciones iniciales que indiquen claramente el tema, naming los actores señalados en el reactivo (por ejemplo: "Especialistas en medicina"), el contexto espacial explícito (por ejemplo: "en las grandes ciudades") y un marcador temporal concreto (por ejemplo: "en la actualidad" o "en las últimas décadas").</t>
         </is>
       </c>
       <c r="C13" s="2" t="inlineStr">
         <is>
-          <t>La conclusión reformula la idea principal (que las medidas gubernamentales inducirán un cambio de actitud que reducirá la contaminación) y plantea una proyección clara sobre consecuencias positivas para el ambiente y la salud, por lo que cumple síntesis y proyección y responde al reactivo al priorizar acciones estructurales sobre el autocuidado individual. Deficiencias: formulación repetitiva y vaga («granito de arena»), faltan referencias explícitas a los argumentos de especialistas y precisión sobre qué medidas y plazos, además de errores de redacción que afectan la claridad.</t>
+          <t>La conclusión presenta un cierre claro que reafirma la tesis central (que el gobierno debe implementar medidas para incentivar conductas que reduzcan la contaminación) y además proyecta consecuencias futuras relevantes (que la suma de cambios individuales reducirá la contaminación y mejorará la salud), por lo que cumple síntesis y proyección y responde al reactivo. Deficiencias: repite la tesis con escasa reformulación conceptual y sin integrar explícitamente el contraste planteado por el reactivo respecto al autocuidado/actividad física; usa cuantificaciones vagas («la mayoría», «granito de arena») y contiene imprecisiones y errores de estilo que debilitan la contundencia de la proyección.</t>
         </is>
       </c>
       <c r="D13" s="2" t="inlineStr">
         <is>
-          <t>El texto tiene párrafos identificables y utiliza conectores lógicos (“En primer lugar”, “En segundo lugar”, “Si bien”, “Así, podemos concluir”), además responde al reactivo al proponer medidas gubernamentales. Sin embargo, presenta repetición en dos párrafos: el párrafo 3 retoma la idea general de la introducción sobre el daño de la contaminación para la salud (ya afirmada en el primer párrafo), y el párrafo 5 (conclusión) repite argumentos e imágenes ya expuestos en los párrafos 2 y 4 acerca del efecto acumulativo de pequeñas acciones y el cambio de conducta por incentivos. Esa repetición en dos párrafos corresponde exactamente al criterio de NIVEL 2.</t>
+          <t>El texto presenta párrafos claramente identificables y conectores lógicos ('En primer lugar', 'En segundo lugar', 'Si bien', 'Así'). Los subtemas son distinguibles: (1) introducción y tesis; (2) incentivo al transporte público; (3) campañas contra el tabaquismo/uso de mascarillas; (4) refutación de la objeción sobre el cambio de conducta; (5) conclusión. No obstante, hay repetición: el párrafo 5 (conclusión) repite la idea central ya expuesta en los párrafos 2 y 4 —que las medidas gubernamentales e incentivos individuales, al sumarse, reducirán la contaminación—, por lo que existe al menos un párrafo que repite información previa. Además, la respuesta al reactivo es solo parcial: si bien el autor pide medidas gubernamentales, no aborda con precisión la afirmación clave de los especialistas (que las medidas individuales no inciden eficazmente en las condiciones que generan la contaminación) ni propone medidas estructurales claras que cambien esas condiciones. Según la escala y la presencia de una repetición entre párrafos, corresponde 2 puntos.</t>
         </is>
       </c>
     </row>
@@ -668,10 +668,10 @@
         <v>4</v>
       </c>
       <c r="B14" s="2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C14" s="2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D14" s="2" t="n">
         <v>2</v>
@@ -681,17 +681,17 @@
       <c r="A15" s="2" t="n"/>
       <c r="B15" s="2" t="inlineStr">
         <is>
-          <t>El texto introduce el tema central (la necesidad de acciones mayores que las individuales para mejorar la salud frente a la contaminación en grandes ciudades) y menciona actores relevantes (políticas públicas, gobierno, colectivos) y un ámbito espacial general (</t>
+          <t>Hay presente el qué (la necesidad de eliminar condiciones que afectan la salud en las grandes ciudades) y el dónde (las grandes ciudades) y se mencionan actores generales (políticas públicas, gobierno, colectivos, personas), pero falta el cuándo: no hay periodo temporal ni marco histórico. Además los 'quiénes' son vagos (grupos generales, no actores concretos ni especialistas como plantea el reactivo). La oración inicial es larga y equivoca a una introducción completa.</t>
         </is>
       </c>
       <c r="C15" s="2" t="inlineStr">
         <is>
-          <t>El cierre contiene una síntesis explícita de la tesis central: que el cambio debe estar en manos de algo mayor que el individuo (políticas públicas y colectivos) y reconoce la importancia de acciones individuales. No obstante, falla en ofrecer una proyección clara: no expone consecuencias concretas, pasos futuros, políticas propuestas ni implicaciones prácticas o temporales. La proyección aparece tenue y repetitiva en forma de deseo general (</t>
+          <t>Existe una síntesis: se reitera la idea central (los cambios deben ser colectivos, apoyados por políticas y cultura social). Sin embargo la proyección es débil o inexistente: no ofrece consecuencias claras, recomendaciones concretas ni escenarios futuros; simplemente repite la tesis. Tampoco articula cómo las implicaciones responden al matiz del reactivo sobre el papel del autocuidado frente a las acciones estructurales.</t>
         </is>
       </c>
       <c r="D15" s="2" t="inlineStr">
         <is>
-          <t>La estructura textual presenta intentos de organización (</t>
+          <t>Hay conectores básicos (En primer lugar, En segundo lugar, Pero, En conclusión) y se presentan subtemas (políticas públicas, cultura social, contraargumento individual), pero el texto repite ideas: la necesidad de acción colectiva/políticas aparece en varias secciones y la conclusión vuelve a reiterarla sin aportar nueva información. Algunos párrafos mezclan subtemas (ejemplo de bolsas, gases, salud) y hay redundancia entre párrafos (especialmente tesis inicial, desarrollo sobre políticas y cierre), lo que debilita la progresión.</t>
         </is>
       </c>
     </row>
@@ -701,27 +701,27 @@
         <v>2</v>
       </c>
       <c r="C16" s="2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D16" s="2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="n"/>
       <c r="B17" s="2" t="inlineStr">
         <is>
-          <t>Se identifican 2 elementos claros: 1) Qué: tema central presente (la necesidad de acciones colectivas/políticas para mejorar la salud en las grandes ciudades) aunque expresado de forma extensa y poco condensada; 2) Dónde: aparece el contexto espacial (las grandes ciudades) y se dan ejemplos específicos (Chile, India). Faltan o son insuficientes los otros dos elementos exigidos: Quiénes aparece de manera vaga ("el gobierno", "un colectivo", "las personas"), sin actores concretos por nombre o instituciones precisas; Cuándo está ausente (no hay periodo, fecha ni marco temporal definido, solo referencias generales como "diariamente"). Además, la introducción no señala explícitamente el contraste planteado en el reactivo (la postura de especialistas sobre el autocuidado frente a las medidas estructurales), por lo que su pertinencia respecto al reactivo es incompleta. Por estas deficiencias (ausencia de Quiénes específicos y de Cuándo, y falta de mención explícita de la posición de los especialistas), corresponde NIVEL 2.</t>
+          <t>Pertinencia: el texto responde al reactivo al contrastar acciones individuales con políticas públicas y acción colectiva frente a la contaminación urbana. Qué: el tema (la insuficiencia de acciones individuales y la necesidad de políticas/colectivos para proteger la salud en ciudades) aparece pero no se expresa de forma clara y concisa en 1–2 oraciones. Quiénes: aparecen actores generales («gobierno», «políticas públicas», «colectivo», «personas»), pero no se nombran actores concretos ni instituciones específicas (p. ej. ministerios, gobiernos locales, organizaciones civiles) —esto lo hace vago. Dónde: hay referencia al contexto espacial general («grandes ciudades») y ejemplos por país (Chile, India), pero la introducción no fija un ámbito geográfico específico y coherente como requeriría mayor precisión. Cuándo: no hay ningún periodo temporal, fecha o marco histórico explícito. Para alcanzar 3 puntos haría falta: a) una definición concisa del tema en 1–2 oraciones, b) nombrar actores concretos e identificables, y c) añadir un marco temporal claro.</t>
         </is>
       </c>
       <c r="C17" s="2" t="inlineStr">
         <is>
-          <t>El texto presenta un cierre a modo de comentario que retoma la tesis central (que las soluciones deben trascender la acción individual y requerir políticas públicas y cultura colectiva) por lo que responde al reactivo de forma general. Sin embargo, la síntesis es débil: no reformula la idea principal con palabras significativamente nuevas, sino que repite y amalgama información ya expuesta. La proyección también es insuficiente: ofrece afirmaciones generales (las acciones individuales pueden inspirar políticas o cultura) pero carece de implicaciones concretas, consecuencias futuras o escenarios relevantes que profundicen la reflexión. En conjunto, funciona como cierre comentario (nivel 3) pero falla en aportar una síntesis renovada y una proyección sólida.</t>
+          <t>La conclusión sí sintetiza la idea central del reactivo: que los cambios reales deben ser colectivos y apoyados por políticas públicas, reconociendo además el papel catalizador de las acciones individuales. Sin embargo, falla en la proyección: no plantea implicaciones concretas, consecuencias claras ni escenarios o recomendaciones futuras relevantes; se limita a reiterar la tesis de forma vaga y repetitiva. Responde al reactivo pero carece del cierre prospectivo exigido.</t>
         </is>
       </c>
       <c r="D17" s="2" t="inlineStr">
         <is>
-          <t>Aunque se reconocen párrafos identificables y hay conectores ('En primer lugar', 'En segundo lugar', 'Pero', 'En conclusión'), la progresión es deficiente porque varios párrafos repiten la misma idea central (la necesidad de acciones más allá del individuo) en lugar de desarrollar subtemas distintos. Específicamente: el párrafo 3 (ejemplo/ consecuencias de Chile/India) vuelve a repetir y ampliar lo ya señalado en el párrafo 2 sobre prácticas colectivas; el párrafo 4 (contraargumento sobre acciones individuales que generan cambio) retoma y contradice sin aportar un subtema nuevo lo expuesto en los párrafos 1 y 2; el párrafo 5 (conclusión) reitera la tesis general sin añadir síntesis o implicaciones nuevas. Además, aunque hay conectores, no generan una progresión lógica que avance la argumentación; varias ideas se repiten en más de dos párrafos. Por tanto, según la escala, corresponde NIVEL 1.</t>
+          <t>El texto presenta cuatro párrafos identificables con conectores claros ("En primer lugar", "En segundo lugar", "Pero", "En conclusión") y responde al reactivo al plantear la necesidad de medidas sociales/sistémicas y la aportación limitada de acciones individuales. Sin embargo, hay repetición de ideas: el párrafo final (conclusión) reitera sin aportar un subtema nuevo las mismas proposiciones ya desarrolladas en los párrafos anteriores (políticas públicas, acción colectiva y la mención de cambios individuales). No se observan dos párrafos distintos que digan básicamente lo mismo, pero sí hay al menos un párrafo que repite información previa, por lo que corresponde 2 puntos.</t>
         </is>
       </c>
     </row>
@@ -730,10 +730,10 @@
         <v>5</v>
       </c>
       <c r="B18" s="2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C18" s="2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D18" s="2" t="n">
         <v>3</v>
@@ -743,27 +743,27 @@
       <c r="A19" s="2" t="n"/>
       <c r="B19" s="2" t="inlineStr">
         <is>
-          <t>El texto identifica claramente el tema central (límites entre expresión artística y respeto a la autoridad) y menciona actores relevantes (el colectivo Las Tesis y, de forma general, Carabineros). Sin embargo falta información espacial específica (no dice que ocurre en Chile ni ubica el conflicto en un contexto geográfico preciso) y no indica un periodo temporal o momento histórico concreto vinculado al reactivo. Es, por tanto, parcial: Qué y Quiénes están presentes; Dónde y Cuándo ausentes.</t>
+          <t>El texto incluye claramente el "qué" (controversia sobre las actividades de Las Tesis) y el "quiénes" (el colectivo Las Tesis y Carabineros), pero carece de "dónde" y "cuándo": no especifica el contexto espacial (no menciona explícitamente Chile ni el ámbito jurisdiccional) ni el periodo o momento temporal de los hechos. Además no incorpora datos concretos del reactivo (la denuncia legal, el video con la consigna citada) que permitirían una introducción completa y situada.</t>
         </is>
       </c>
       <c r="C19" s="2" t="inlineStr">
         <is>
-          <t>Hay una síntesis clara: reafirma que la libertad de expresión es esencial y que sus límites deben ser excepcionales y ex post. No obstante, la proyección es vaga y genérica: ofrece una recomendación normativa (preferir control ex post) pero no desarrolla consecuencias concretas, implicaciones legales ni acciones futuras específicas relacionadas con el caso citado en el reactivo. Falta concreción y vínculo explícito con medidas o escenarios futuros.</t>
+          <t>Hay una síntesis clara: se reitera que la libertad de expresión es esencial y que las limitaciones deben ser ex post. También hay una proyección general (la sociedad debe valorar la libertad como piedra angular). Sin embargo, la proyección es vaga y retórica: no ofrece implicaciones concretas, consecuencias normativas ni criterios aplicables al caso (por ejemplo sobre la denuncia penal, la distinción arte/no-arte o requisitos para sancionar). Para alcanzar puntaje máximo debería formular consecuencias precisas y relacionarlas con el caso planteado.</t>
         </is>
       </c>
       <c r="D19" s="2" t="inlineStr">
         <is>
-          <t>La estructura en párrafos es clara y hay conectores («En primer lugar», «En segundo lugar», «Otros podrían sostener...»). No obstante, existe redundancia parcial: el párrafo sobre censura y arbitrariedad (párrafo 2) y el que analiza el riesgo de control previo por la autoridad (párrafo 4) reiteran la misma preocupación con argumentos similares; además el desarrollo sobre la función de la libertad de expresión (párrafo 3) repite parcialmente la defensa normativa ya planteada. En conjunto aporta coherencia, pero hay repetición conceptual que impide nivel máximo.</t>
+          <t>Estructuralmente los párrafos aportan subtemas distintos (presentación del conflicto; argumento contra la censura y riesgo de arbitrariedad; defensa de la disidencia; consideración del contraargumento de Popper y ponderación). Hay conectores lógicos y no hay repetición literal. No obstante, aunque la progresión formal es buena, el texto no desarrolla aspectos centrales del reactivo (ausencia de análisis sobre la denuncia específica, la frase citada, la distinción práctica entre expresión artística y conducta punible y la doctrina del "peligro"), por lo que, pese a la buena organización, falta profundizar en los elementos que debería tratar.</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="2" t="n"/>
       <c r="B20" s="2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C20" s="2" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D20" s="2" t="n">
         <v>2</v>
@@ -773,17 +773,17 @@
       <c r="A21" s="2" t="n"/>
       <c r="B21" s="2" t="inlineStr">
         <is>
-          <t>La introducción cumple con el 'qué' (el límite entre expresión artística y respeto a la autoridad) y con los 'quiénes' (menciona al colectivo Las Tesis y a Carabineros), por lo que es parcialmente pertinente al reactivo. Sin embargo faltan el 'dónde' (no se indica explícitamente la ubicación geográfica, p. ej. que el conflicto ocurre en Chile) y el 'cuándo' (no hay fecha, periodo o momento histórico concreto ni referencia precisa a la denuncia reciente). Además no se nombra con exactitud la denuncia y los cargos apuntados en el reactivo. Para alcanzar NIVEL 4, la introducción debe añadir en 1–2 oraciones específicas la ubicación geográfica y un periodo/fecha precisos, y mencionar brevemente la denuncia legal señalada en el reactivo (sin inventar datos).</t>
+          <t>Qué: Presente y relativamente específico (límite entre expresión artística y respeto a la autoridad). Quiénes: Presentes y concretos (colectivo Las Tesis; se alude a Carabineros). Dónde: Ausente; no hay ubicación geográfica ni contexto espacial (no se menciona Chile, ciudad ni ámbito institucional concreto). Cuándo: Ausente; no hay referencia temporal ni indicación de que se trata de la denuncia reciente señalada en el reactivo. Además, la introducción no sitúa la controversia en el marco preciso del reactivo (denuncia legal concreta, cargos como atentado contra la autoridad/amenazas y la polémica sobre el supuesto riesgo que justificaría limitar la expresión artística), por lo que faltan datos esenciales para cumplir los cuatro elementos exigidos.</t>
         </is>
       </c>
       <c r="C21" s="2" t="inlineStr">
         <is>
-          <t>La conclusión reformula con claridad la idea central (la libertad de expresión como bien esencial y la preferencia por límites ex post) cumpliendo la síntesis exigida, y además plantea proyección al señalar las implicaciones democráticas y la necesidad social de revalorar la libertad ante intervenciones artísticas como las de Las Tesis. Es pertinente respecto al reactivo porque aborda directamente el conflicto entre expresión artística y restricción preventiva. Observaciones menores: la proyección queda algo general y podría beneficiarse de implicaciones más concretas (p. ej. criterios normativos o consecuencias jurídicas), y el último enunciado resulta algo redundante.</t>
+          <t>Cumple síntesis: reformula la idea principal (prioridad de la libertad de expresión y que sus límites deben fundarse en razones relevantes) en palabras nuevas. Cumple proyección: plantea una preferencia normativa (límites ex post) y convoca a la sociedad a reevaluar la libertad de expresión, lo que constituye una reflexión prospectiva pertinente al reactivo. Debilidades: el cierre es algo genérico y no desarrolla consecuencias concretas ni medidas específicas frente a la denuncia de Carabineros, por lo que podría fortalecer la proyección vinculándola más directamente con escenarios legales o sociales futuros.</t>
         </is>
       </c>
       <c r="D21" s="2" t="inlineStr">
         <is>
-          <t>Los párrafos son claramente identificables y hay conectores lógicos ("En primer lugar", "En segundo lugar", "Otros podrían sostener", "En conclusión"). Sin embargo, se detectan repeticiones en dos párrafos: el párrafo 4 (el contraargumento sobre el peligro del control previo y la arbitrariedad de la autoridad, referencia a Popper) repite en esencia la preocupación ya expuesta en el párrafo 2 sobre la arbitrariedad y el riesgo del control previo; y el párrafo 5 (conclusión que defiende límites ex post y resalta la centralidad de la libertad de expresión) rehace la preferencia por el control ex post y la defensa de la libertad que ya se plantea en el párrafo 4 y en pasajes anteriores. El texto sí responde al reactivo (defiende una libertad de expresión artística amplia y la preferencia por límites ex post), pero la redundancia en los párrafos señalados impide una progresión plenamente diferenciada de ideas, por lo que corresponde NIVEL 2.</t>
+          <t>El texto tiene párrafos claramente identificables y conectores lógicos ("En primer lugar", "En segundo lugar", "Otros podrían...", "En conclusión") y responde al reactivo defendiendo la primacía de la libertad de expresión artística salvo razones muy relevantes. Sin embargo, hay repetición de ideas: el párrafo 2 (sobre censura, arbitrariedad y peligro del control por la autoridad) y el párrafo 4 (que plantea la disyuntiva entre control ex ante por la autoridad y permitir que se abogue por limitar la libertad) transmiten esencialmente la misma preocupación acerca del riesgo del control previo y la arbitrariedad; esto constituye una repetición de contenido entre dos párrafos. El párrafo 3 trata un subtema próximo (la función de la libertad de expresión para garantizar la disidencia) y es distinto, aunque afín al argumento general. Para alcanzar puntaje 3 bastaría con eliminar o reformular brevemente el párrafo 4 para que aporte un elemento nuevo (por ejemplo, desarrollar específicamente la referencia a Popper como una preocupación distinta: mecanismo de autolimitación social o criterios para sanciones ex post), evitando repetir la tesis sobre la arbitrariedad del control ex ante.</t>
         </is>
       </c>
     </row>
@@ -792,60 +792,60 @@
         <v>6</v>
       </c>
       <c r="B22" s="2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C22" s="2" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D22" s="2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="2" t="n"/>
       <c r="B23" s="2" t="inlineStr">
         <is>
-          <t>El tema central (teletrabajo y pandemia) y un indicador temporal ('Hoy en día', 'covid-19') están presentes, pero los demás elementos son vagos: los 'quiénes' se limitan a 'muchas personas' sin identificar actores o grupos relevantes por nombre, y el 'dónde' es solo 'en todo el mundo' (contexto demasiado general). Además no conecta explícitamente con el aspecto específico del reactivo (la noción del hogar como refugio en peligro). Se requiere mayor especificidad en actores, contexto espacial y vínculo directo con el problema planteado en el reactivo.</t>
+          <t>El texto menciona el tema central (pandemia y teletrabajo) y un grupo afectado ("muchas personas en todo el mundo") y el marco temporal (la pandemia por covid-19), pero varios elementos son vagos. "Quiénes" aparece como un grupo genérico sin actores concretos (no se identifican tipos de trabajadores, instituciones o colectivos), "dónde" se limita a "en todo el mundo" (contexto demasiado general) y "cuándo" usa expresiones vagas como "Hoy en día" en lugar de un periodo concreto. Para alcanzar puntaje máximo serían necesarias referencias más específicas sobre actores y un acotamiento espacial y temporal más preciso.</t>
         </is>
       </c>
       <c r="C23" s="2" t="inlineStr">
         <is>
-          <t>Hay una formulación sintética breve ('el encierro... han generado un alto impacto en la salud mental'), que resume la consecuencia principal, pero falta totalmente proyección: no hay implicaciones, recomendaciones, reflexiones futuras ni cierre conceptual. La síntesis es mínima y no sustituye una conclusión que reformule en otras palabras y proyecte consecuencias o soluciones.</t>
+          <t>No existe una conclusión ni cierre: el texto termina señalando un problema (impacto en la salud mental) pero no reformula la idea principal ni ofrece proyección, implicaciones o reflexiones futuras. Falta síntesis en términos propios y una proyección sobre consecuencias, recomendaciones o líneas de investigación/acción.</t>
         </is>
       </c>
       <c r="D23" s="2" t="inlineStr">
         <is>
-          <t>El texto consta de un solo párrafo corto que combina introducción y consecuencia; no hay desarrollo en párrafos separados ni progreso temático claro. Las dos oraciones aportan información relacionada pero limitada y en parte redundante (teletrabajo por pandemia → impacto en salud mental), faltan conectores que expliquen la transición y no se explora la noción específica del hogar como refugio, por lo que la progresión es insuficiente. Se recomienda dividir en párrafos distintivos (contexto, problema específico, evidencia/ejemplos, cierre) y añadir conectores y desarrollo del aspecto solicitado por el reactivo.</t>
+          <t>El texto está compuesto por un solo bloque breve y no hay desarrollo de subtemas en párrafos diferenciados. La segunda frase apenas reitera y amplía la primera (encierro y sobrecarga → impacto en salud mental) sin aportar información nueva sustantiva ni conectores que organicen la progresión. Se requieren párrafos distintos (contexto, problema específico, evidencia/ejemplos, implicaciones) y mejores conectores para evitar esta falta de estructura y redundancia.</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="2" t="n"/>
       <c r="B24" s="2" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C24" s="2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D24" s="2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="2" t="n"/>
       <c r="B25" s="2" t="inlineStr">
         <is>
-          <t>La introducción presenta el Qué (impacto en la salud mental por teletrabajo) y el Cuándo (la pandemia por COVID-19), pero falla en Quiénes y Dónde: los actores están descritos de forma genérica («muchas las personas», «personas que trabajan desde sus casas») en lugar de identificar grupos concretos (por ejemplo, trabajadores de la salud, docentes, empleados de empresas privadas, padres que teletrabajan), y la ubicación es demasiado general («en todo el mundo», «desde sus casas») en lugar de precisar un contexto espacial (país, región, ciudad o contexto institucional). Además, aunque aborda la salud mental, no incorpora de manera explícita la idea central del reactivo sobre el hogar como espacio/ refugio amenazado. Para alcanzar Nivel 4 se requiere nombrar actores específicos, acotar la ubicación espacial y precisar el periodo (por ejemplo, pandemia de COVID-19 con años) y aludir claramente al riesgo sobre el hogar como lugar protegido.</t>
+          <t>Solo presenta claramente el "qué" (impacto en la salud mental por el teletrabajo) y el "cuándo" (durante la pandemia de covid-19). Falta el elemento "quiénes" concreto: se habla de "muchas personas" y "personas que trabajan desde sus casas" de forma genérica, sin identificar actores o grupos específicos (p. ej. teletrabajadores de sectores determinados, empleadores, familias, autoridades sanitarias). También falta un "dónde" específico: "en todo el mundo" es vago y no aporta una ubicación geográfica o contexto espacial preciso (país, ciudad, ámbito doméstico concreto). Además, la introducción no alude explícitamente al aspecto central del reactivo sobre la casa como último refugio puesto en peligro. Por ello no cumple los cuatro elementos exigidos.</t>
         </is>
       </c>
       <c r="C25" s="2" t="inlineStr">
         <is>
-          <t>El fragmento ofrece un cierre a modo de comentario y resume de forma general la situación (síntesis superficial), pero no plantea proyecciones, implicaciones ni reflexiones futuras. Además no atiende con precisión el núcleo del reactivo: la amenaza al hogar como último refugio; el cierre es descriptivo y escaso, sin análisis prospectivo.</t>
+          <t>La sección final funciona como un comentario que resume el problema (síntesis mínima presente) pero carece totalmente de proyección: no plantea implicaciones, consecuencias ni reflexiones futuras. Además no responde al énfasis del reactivo sobre el hogar como refugio ni sugiere medidas, políticas o líneas de acción para proteger ese espacio. Sugerencia breve: añadir una frase que proyecte consecuencias y acciones (por ejemplo, la necesidad de normas claras, apoyo institucional y estrategias para preservar el hogar como espacio de descanso) para alcanzar puntaje máximo.</t>
         </is>
       </c>
       <c r="D25" s="2" t="inlineStr">
         <is>
-          <t>El texto consta de un único párrafo, por lo que no existe progresión entre párrafos ni conectores interparagraphales; no se cumplen los tres criterios exigidos (no hay párrafos con subtemas distintos, no puede evaluarse ausencia de repetición entre párrafos y falta de conectores). Además, el contenido responde parcialmente al reactivo: habla de teletrabajo y salud mental, pero no aborda la idea central planteada (la amenaza a la noción del hogar como refugio). Por estas deficiencias claras y específicas, corresponde Nivel 1.</t>
+          <t>El texto consta de un solo párrafo, por lo que no puede evaluarse una progresión entre párrafos ni la presencia de subtemas distintos. No hay conectores interparrafales y falta estructura (no hay varios párrafos con información secuenciada). Además, aunque el párrafo menciona teletrabajo y afectación de la salud mental, no responde plenamente al reactivo central (la 'salud del hogar' como refugio amenazado) ni desarrolla subtemas distintos; por tanto no cumple los criterios exigidos.</t>
         </is>
       </c>
     </row>
@@ -854,60 +854,60 @@
         <v>7</v>
       </c>
       <c r="B26" s="2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C26" s="2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D26" s="2" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="2" t="n"/>
       <c r="B27" s="2" t="inlineStr">
         <is>
-          <t>El párrafo inicial declara el tema general (políticas educativas y diversidad cultural) y sitúa temporalmente ('actualmente'), pero no cumple los cuatro elementos requeridos: no identifica actores concretos (p. ej. estudiantes inmigrantes, Ministerio de Educación, docentes, familias) ni especifica el lugar más allá de un vago 'nuestro país'. Tampoco menciona explícitamente el sujeto central del reactivo (estudiantes inmigrantes) en la entrada. Para mejorar: incluir en una o dos oraciones el qué (inclusión de estudiantes inmigrantes), quiénes (actores específicos) y el dónde (país/ contexto escolar) con periodo temporal concreto.</t>
+          <t>La apertura no cumple los cuatro elementos exigidos. Hay una idea general del 'qué' (políticas educativas y diversidad cultural) y una indicación temporal vaga ('actualmente'), pero faltan actores identificados (no se nombran explícitamente 'estudiantes inmigrantes', autoridades, docentes ni grupos opositores por nombre) y el 'dónde' es genérico ('nuestro país') sin especificidad contextual. Además no se enuncia con claridad el problema concreto planteado en el reactivo (si los inmigrantes deben adecuarse o si su inclusión amenaza valores nacionales). Sugiero reescribir la introducción indicando claramente: 1) el tema en una frase precisa vinculada al reactivo, 2) los actores relevantes (estudiantes inmigrantes, comunidad escolar, Estado), 3) el contexto espacial (país o sistema educativo específico) y 4) el periodo temporal (por ejemplo, 'en la actualidad' ampliado con fechas o marco político).</t>
         </is>
       </c>
       <c r="C27" s="2" t="inlineStr">
         <is>
-          <t>El cierre ofrece un enunciado normativo general sobre la finalidad de la educación, pero no sintetiza claramente la idea principal del ensayo ni reformula en palabras nuevas el argumento respecto al reactivo (si los inmigrantes deben adecuarse o integrarse). Tampoco plantea proyecciones explícitas, consecuencias políticas o recomendaciones concretas. Hay intento de cierre retórico, pero carece de síntesis estructurada y de implicaciones operativas; se requiere una oración que resuma la posición frente al reactivo y otra que indique consecuencias o pasos futuros.</t>
+          <t>El cierre es un intento normativo pero no cumple las funciones requeridas: no sintetiza la idea principal del ensayo ni reformula argumentos centrales relativos al reactivo (no resume la posición sobre adaptación versus inclusión cultural), y tampoco ofrece proyecciones claras (consecuencias políticas, educativas o propuestas concretas). En su lugar presenta una afirmación general sobre valores educativos. Para mejorar: incluir una frase que reformule la tesis con nuevas palabras y añadir al menos una proyección concreta (implicaciones para la política curricular, prácticas docentes o investigación futura).</t>
         </is>
       </c>
       <c r="D27" s="2" t="inlineStr">
         <is>
-          <t>La secuencia presenta conectores ('Sin embargo', 'No obstante', 'Por otro lado'), pero hay solapamiento temático: el primer y el tercer párrafo repiten parcialmente la idea sobre políticas educativas y la inclusión (información redundante en distinta formulación). Asimismo, los párrafos que defienden la integración y los que abogan por preservar tradiciones se superponen sin una progresión clara entre argumento y contraargumento. Falta claridad en temas por párrafo y en la delimitación de subtemas; recomendar reorganizar para que cada párrafo desarrolle un único subtema (contexto/políticas, postura conservadora, estado real de la inclusión, argumentos a favor de la integración, argumentos a favor de preservar tradiciones, conclusión).</t>
+          <t>La progresión textual es débil y redundante: varios párrafos repiten temas sin desarrollar subtemas distintos (p. ej. la defensa de tradiciones aparece en los párrafos 2 y 5; la diferencia entre 'invitación' e 'integración' aparece en el párrafo 1 y se retoma en el 3; las valoraciones personales 'creo' se repiten en 4 y 5 sin mayor distinción). Faltan conectores lógicos que articulen causa-efecto o contraste de modo claro; la estructura carece de desarrollo secuenciado de argumentos y algunos enunciados son discursivamente aislados. Para corregir: reorganizar para que cada párrafo aborde un subtema único (contexto/políticas; argumentos en contra; prácticas reales; beneficios de la integración; límites y propuestas) y añadir transiciones que muestren la relación entre ellos, eliminando repeticiones.</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="2" t="n"/>
       <c r="B28" s="2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C28" s="2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D28" s="2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="2" t="n"/>
       <c r="B29" s="2" t="inlineStr">
         <is>
-          <t>Solo el "Qué" está claramente presente: el tema son las políticas educativas y la inclusión cultural en los establecimientos. "Quiénes" aparecen de forma genérica ("un gran porcentaje de la población", "comunidades inmigrantes", "familias") pero no hay actores concretos por nombre. "Dónde" es vago: dice "nuestro país" sin identificar qué país ni contexto educativo específico. "Cuándo" solo aparece como "actualmente", sin periodo o fechas precisas. Respecto al reactivo, el texto alude a la postura contraria pero no especifica quién la sostiene ni en qué contexto espacial/temporal. Para llegar a NIVEL 4 se necesita: 1) en 1–2 oraciones iniciales formular el tema claramente; 2) sustituir "nuestro país" por el nombre del país o contexto geográfico preciso; 3) nombrar actores concretos (por ejemplo: Ministerio de Educación, directores, padres conservadores, estudiantes inmigrantes); y 4) precisar el periodo temporal (año, rango o marco histórico).</t>
+          <t>Solo cumple claramente 1 elemento: Qué (tema central: políticas educativas e inclusión cultural de estudiantes inmigrantes). Los otros tres elementos son vagos o inexistentes: Quiénes — se alude a “un gran porcentaje de la población”, “familias” y “comunidades inmigrantes” pero no hay actores concretos nombrados; Dónde — solo aparece “nuestro país”, sin identificación geográfica específica; Cuándo — la única marca temporal es “actualmente”, demasiado general para considerarse un periodo o fecha precisa. Respecto al reactivo, el texto es pertinente porque aborda la tensión entre adaptación cultural e inclusión, pero falla en especificar actores, lugar y tiempo necesarios para una introducción académica completa y específica.</t>
         </is>
       </c>
       <c r="C29" s="2" t="inlineStr">
         <is>
-          <t>El cierre del texto funciona como comentario y reflexión (proyección): propone consecuencias y prácticas educativas (integración enriquecedora, preservar tradiciones en primeros años, promover colaboración). Sin embargo, falla en la síntesis: no reformula de manera clara y concisa la idea principal del ensayo sobre el debate entre asimilación e inclusión; la conclusión está dispersa en varios párrafos y ofrece recomendaciones más que una conclusión que recoja y reformule la tesis. Aunque pertinente al reactivo, la falta de una reformulación explícita de la tesis impide un nivel superior.</t>
+          <t>La sección final contiene comentarios y proyecciones (integración enriquecedora, preservación de tradiciones en primeros años, cambio de la educación hacia la colaboración), pero no ofrece una síntesis clara y reformulada de la idea principal del texto ni responde de modo explícito y directo al reactivo. La conclusión está fragmentada en varios párrafos y mayormente enunciativa: predominan opiniones y deseos generales en lugar de una reformulación concisa de la tesis (falta la síntesis exigida). La proyección existe pero es parcial y poco articulada con la tesis central (no se aclara de forma contundente si y cómo deben adaptarse los estudiantes inmigrantes frente a la conservación cultural nacional). En conjunto, funciona como cierre a modo de comentario más que como una conclusión que sintetice y proyecte plenamente.</t>
         </is>
       </c>
       <c r="D29" s="2" t="inlineStr">
         <is>
-          <t>Los párrafos son claramente identificables y hay conectores lógicos entre ellos; además el texto responde al reactivo al presentar políticas educativas, la postura conservadora contraria y argumentos a favor de la integración con cautelas sobre la preservación de tradiciones. Sin embargo existe repetición de ideas: el párrafo 4 (ventajas de una integración realmente efectiva) y el párrafo 5 (defensa de la integración junto con la preservación de tradiciones) comunican esencialmente el mismo argumento sobre los beneficios de la integración intercultural; además el párrafo 3 retoma de forma muy cercana el tema de la inclusión ya mencionado en el párrafo 1 (política curricular), aunque con distinto énfasis en implementación. Por existir al menos un párrafo que repite información de uno anterior, corresponde NIVEL 3.</t>
+          <t>Los párrafos son identificables y el texto responde al reactivo (presenta postura conservadora, análisis de políticas e posición a favor de integración respetuosa). Hay conectores lógicos entre párrafos ("Sin embargo", "No obstante", "Por otro lado", "Para ir finalizando"). Sin embargo, existe repetición de ideas: el párrafo 4 (beneficios de una integración efectiva) y el párrafo 5 (necesidad de preservar valores/tradiciones y comparar con comunidades inmigrantes) solapan contenido sobre integración y enriquecimiento cultural; además, el párrafo 1 (marco de políticas) y el párrafo 3 (crítica a la implementación de la inclusión) abordan la misma dimensión normativa y podrían leerse como reiterativos. Para alcanzar puntaje 3 se requiere una corrección mínima: condensar o distinguir claramente el enfoque del párrafo 4 y 5 (por ejemplo, dejar el párrafo 4 centrado exclusivamente en los beneficios de la integración y el párrafo 5 exclusivamente en la defensa de la transmisión de tradiciones y su articulación con la inclusión inmigrante), y precisar que el párrafo 3 añade evidencia o ejemplo concreto que no repita literalmente el marco presentado en el párrafo 1.</t>
         </is>
       </c>
     </row>
@@ -916,60 +916,48 @@
         <v>8</v>
       </c>
       <c r="B30" s="2" t="n">
-        <v>3</v>
-      </c>
-      <c r="C30" s="2" t="n">
-        <v>4</v>
-      </c>
-      <c r="D30" s="2" t="n">
-        <v>3</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="C30" s="2" t="n"/>
+      <c r="D30" s="2" t="n"/>
     </row>
     <row r="31">
       <c r="A31" s="2" t="n"/>
       <c r="B31" s="2" t="inlineStr">
         <is>
-          <t>La introducción contiene el qué (teletrabajo y salud mental), el dónde (Chile) y una referencia temporal general (la pandemia/«antes de la pandemia»), pero adolece de especificidad: los actores aparecen de forma genérica («los trabajadores», «las personas») en lugar de identificarse con mayor precisión y el marco temporal es vago (no hay fechas ni periodo concreto). Además hay un inicio fraccionado («Siendo esta...») que debilita la presentación. En conjunto, faltan precisión y concreción que evitarían ambigüedades respecto al reactivo.</t>
-        </is>
-      </c>
-      <c r="C31" s="2" t="inlineStr">
-        <is>
-          <t>La conclusión sintetiza la idea principal (el teletrabajo como solución temporal pero con riesgos para el bienestar psicológico) y ofrece proyección explícita: llama a crear normas y regulaciones y señala la posibilidad de una «nueva normalidad». Aunque hay errores formales menores («por que»), cumple ambas funciones exigidas: síntesis renovada y proyección/implicaciones.</t>
-        </is>
-      </c>
-      <c r="D31" s="2" t="inlineStr">
-        <is>
-          <t>La estructura usa conectores claros («Por una parte», «Por otra parte», «Sin embargo», «Para finalizar»), pero hay repetición temática: el párrafo 2 (hogar como refugio y necesidad de compatibilizar trabajo/hogar) y el párrafo 4 (estrés del trabajo que afecta a la familia) tratan la misma idea central sobre el hogar y el impacto familiar, con solapamiento de contenidos. El párrafo 3 aporta un subtema distinto (contactos fuera de horario) pero sin suficiente desarrollo. En suma, existe al menos un párrafo que repite parcialmente información de otro, por lo que la progresión no es totalmente eficaz.</t>
-        </is>
-      </c>
+          <t>El texto presenta el 'qué' (teletrabajo y su efecto en la salud mental) y el 'dónde' (Chile), y alude al 'cuándo' (</t>
+        </is>
+      </c>
+      <c r="C31" s="2" t="n"/>
+      <c r="D31" s="2" t="n"/>
     </row>
     <row r="32">
       <c r="A32" s="2" t="n"/>
       <c r="B32" s="2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C32" s="2" t="n">
         <v>3</v>
       </c>
       <c r="D32" s="2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="2" t="n"/>
       <c r="B33" s="2" t="inlineStr">
         <is>
-          <t>Se otorga NIVEL 3 porque hay 3 elementos presentes pero al menos uno es vago y falta pertinencia total respecto al reactivo. Lo que sí aparece: (Qué) el tema central —el teletrabajo y su impacto en la salud mental— queda expresado; (Dónde) la ubicación geográfica —Chile— está indicada. Lo que es insuficiente o vago: (Quiénes) solo se menciona de forma general “los trabajadores/las personas” sin identificar con precisión el actor (p. ej. «trabajadores chilenos», «empleados del sector público/privado», o las «familias de teletrabajadores»); (Cuándo) el periodo temporal aparece solo implícito como “situación actual”/“antes de la pandemia” pero no se nombra explícitamente la pandemia por COVID‑19 ni se acota un marco temporal (años/etapas). Además, la introducción no alude directamente al aspecto clave planteado en el reactivo —la noción del hogar como refugio amenazado—, por lo que su pertinencia queda incompleta. Para alcanzar NIVEL 4 se requerirían correcciones mínimas y realistas: en la primera(s) oración(es) nombrar explícitamente «la pandemia por COVID‑19 (2020–2021)», especificar el grupo afectado (por ejemplo «trabajadores chilenos» o «empleados del sector X»), y mencionar que se cuestiona el hogar como lugar protector frente al trabajo remoto.</t>
+          <t>Qué: presente y claro («En este ensayo se sostiene que el teletrabajo amenaza la integridad psicológica de los trabajadores»). Dónde: presente y específico («Chile»). Quiénes: aparecen grupos nombrados («los trabajadores», «empleadores», «familia»), pero son generales; falta precisión sobre qué trabajadores (p. ej. trabajadores chilenos, de qué sector o teletrabajadores concretos). Cuándo: ausente o vago («situación actual»); no se menciona explícitamente la pandemia de COVID‑19 ni un periodo temporal preciso. Por ello falta una de las cuatro piezas requeridas y/o una especificidad suficiente.</t>
         </is>
       </c>
       <c r="C33" s="2" t="inlineStr">
         <is>
-          <t>Existe un cierre identificable que retoma la tesis (el teletrabajo como solución del confinamiento pero con riesgo para la salud mental) y propone una proyección vaga (necesidad de normas/regulaciones y posible 'nueva normalidad'). Sin embargo, la síntesis es débil y en gran parte repetitiva (no reformula con claridad ni añade una conclusión integradora sobre la idea principal) y la proyección es genérica y poco desarrollada (no plantea consecuencias concretas, medidas precisas ni escenarios futuros relevantes). Además hay errores formales ('por que') y falta de precisión que convierten el párrafo final en un comentario con recomendaciones superficiales más que en un cierre analítico y proyectivo completo, por lo que corresponde nivel 3.</t>
+          <t>El cierre distingue una síntesis (reformula la tesis: el teletrabajo protege la continuidad productiva pero amenaza el bienestar psicológico de trabajadores y familias) y una proyección (propone normas/regulaciones y alerta sobre una posible ‘nueva normalidad’). Deficiencias: redacción imprecisa y error ortográfico ('por que' en lugar de 'porque'), las recomendaciones son vagas y no se explicita con fuerza la idea del hogar como último refugio mencionada en el reactivo.</t>
         </is>
       </c>
       <c r="D33" s="2" t="inlineStr">
         <is>
-          <t>El texto presenta párrafos claramente identificables y conectores lógicos ('Por una parte', 'Por otra parte', 'Para finalizar'). Responde al reactivo (pone en cuestión el hogar como refugio y menciona riesgos para la salud mental), pero hay repetición en dos párrafos: el párrafo 4 repite la idea del párrafo 2 sobre cómo el teletrabajo vuelve el hogar un espacio estresante y afecta la convivencia familiar; el párrafo 5 repite la tesis y las recomendaciones ya expuestas (riesgo para el bienestar psicológico y necesidad de normas), replicando información de los párrafos 1–2. Los párrafos 2 y 3 aportan subtemas distintos (protección/educación para compatibilizar hogar-trabajo vs. invasión de tiempo por empleadores), pero la reiteración en 4 y 5 reduce la progresión textual a nivel 2.</t>
+          <t>El texto tiene párrafos identificables y conectores básicos ('Por una parte', 'Por otra parte', 'Para finalizar'), y aborda el reactivo (riesgo del hogar como refugio y salud mental). Sin embargo hay repetición en dos párrafos: el párrafo 4 reproduce la idea central del párrafo 2 (que el hogar puede volverse un ambiente estresante y afectar la vida familiar) y el párrafo 5 reitera la tesis y las mismas consecuencias ya expuestas (riesgo para el bienestar psicológico y familiar). Los subtemas no son siempre claramente distintos: P2 debería centrarse en el hogar como refugio y medidas preventivas; P4 en las consecuencias concretas en la dinámica familiar; P3 en la intrusión del empleador (esa sí distinta). Para alcanzar puntaje 3 bastaría con ajustar brevemente P4 para que trate exclusivamente efectos familiares específicos (evitando repetir la definición del problema) y transformar P5 en una conclusión sintética que no repita contenido previo.</t>
         </is>
       </c>
     </row>
@@ -978,10 +966,10 @@
         <v>9</v>
       </c>
       <c r="B34" s="2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C34" s="2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D34" s="2" t="n">
         <v>3</v>
@@ -991,17 +979,17 @@
       <c r="A35" s="2" t="n"/>
       <c r="B35" s="2" t="inlineStr">
         <is>
-          <t>El texto identifica el qué (salud mental y teletrabajo) y el cuándo (contexto de la pandemia por covid-19) y menciona el lugar en discusión (el hogar), pero falla en especificidad y en la identificación clara de los actores: usa expresiones genéricas («quienes están expuestos al teletrabajo») en lugar de nombrar grupos relevantes (trabajadores, empleadores, autoridades sanitarias, expertos) y no recoge la dimensión señalada en el reactivo de alcance «a nivel mundial». En suma: están presentes los elementos básicos pero son vagos o incompletos.</t>
+          <t>El texto contiene el 'qué' (salud mental y teletrabajo) y el 'cuándo' ('pandemia por el covid-19'), así como una referencia al 'dónde' ('hogar') y a los 'quiénes' ('quienes están expuestos al teletrabajo'). Sin embargo, varios elementos son vagos: los actores no están especificados (no se nombran grupos precisos como trabajadores por sector, empleadores o autoridades), el 'dónde' se queda en el término genérico 'hogar' sin contextualizar tipos de hogares o contextos nacionales/urbanos, y el 'cuándo' es impreciso (menciona la pandemia sin marco temporal concreto). Por tanto, faltan especificidad y concreción exigidas para puntaje máximo.</t>
         </is>
       </c>
       <c r="C35" s="2" t="inlineStr">
         <is>
-          <t>La conclusión cumple parcialmente las funciones: ofrece una síntesis (repite las estrategias propuestas) y una proyección normativa (recomienda que los gobiernos promuevan campañas). Sin embargo, la síntesis es poco reformulada y resulta reiterativa respecto del cuerpo del texto, y la proyección es genérica y no especifica agentes, medios, alcance ni justificación empírica, por lo que no alcanza la completitud exigida para nivel 4.</t>
+          <t>Hay una síntesis explícita de la idea principal (teletrabajo puede realizarse sin perjuicio aplicando estrategias) y una proyección (recomendación a gobiernos de promover campañas). No obstante, la síntesis recicla de forma muy literal las estrategias presentadas y la proyección es vaga: propone una acción gubernamental sin explicitar efectos esperados, destinatarios, condiciones ni pasos concretos. La conclusión es funcional pero insuficientemente desarrollada y poco puntual para alcanzar el puntaje máximo.</t>
         </is>
       </c>
       <c r="D35" s="2" t="inlineStr">
         <is>
-          <t>El texto está organizado en párrafos que abordan subtemas (espacio de trabajo, horarios, ritual de cierre) y emplea conectores. No obstante, hay redundancias parciales: varias secciones repiten la misma idea central de reducir la sensación de trabajo permanente/ansiedad; la contraargumentación y las soluciones reaparecen con alto solapamiento, y la conclusión vuelve a enunciar las mismas estrategias sin aportar información nueva. Además, algunos párrafos quedan poco desarrollados y la cohesión se ve afectada por repeticiones léxicas y errores ortográficos que dificultan la progresión plena.</t>
+          <t>Los párrafos siguen una progresión clara: introducción del problema; desarrollo de tres subtemas diferenciados (espacio definido, respeto de horarios, ritual de cierre) y cierre. Hay conectores ("En primer lugar", "Por otro lado", "Si bien...") que facilitan la coherencia y no hay repetición sustancial entre los párrafos temáticos. La única reiteración notable es la lista de estrategias en la conclusión, que sirve como síntesis y no constituye redundancia entre párrafos temáticos.</t>
         </is>
       </c>
     </row>
@@ -1011,27 +999,27 @@
         <v>2</v>
       </c>
       <c r="C36" s="2" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D36" s="2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="2" t="n"/>
       <c r="B37" s="2" t="inlineStr">
         <is>
-          <t>La introducción contiene 2 de los 4 elementos exigidos: Qué (tema central: preocupación por la salud mental vinculada al teletrabajo y si éste pone en peligro el hogar) y Cuándo (contexto temporal: la pandemia por COVID-19). Faltan los otros dos elementos: Quiénes — los actores aparecen solo de forma genérica («quienes están expuestos al teletrabajo»), no se identifican personas o grupos concretos por nombre; Dónde — no se indica una ubicación geográfica o contexto espacial específico (por ejemplo país, ciudad o la precisión “a nivel mundial” del reactivo). Por tanto la introducción es pertinente al reactivo pero insuficientemente específica en actores y localización, lo que justifica un NIVEL 2.</t>
+          <t>La introducción presenta claramente el Qué (impacto del teletrabajo en la salud mental y la posible puesta en peligro del hogar) y el Cuándo (la pandemia por COVID-19), por lo que esos dos elementos están presentes y relativamente específicos. Sin embargo, falla en el Quiénes: usa expresiones genéricas («quienes están expuestos al teletrabajo») en lugar de identificar grupos concretos (p. ej. trabajadores de oficina, docentes, personal sanitario, teletrabajadores con hijos), y falla en el Dónde: no especifica ubicación geográfica o contexto espacial (p. ej. a nivel nacional, regional o mundial). Debido a que faltan esos dos elementos clave y/o son vagos, la calificación corresponde a 2 puntos.</t>
         </is>
       </c>
       <c r="C37" s="2" t="inlineStr">
         <is>
-          <t>La conclusión reformula de manera clara la idea principal: el teletrabajo puede realizarse sin perjuicio de la salud si se aplican estrategias concretas (síntesis). Además plantea una proyección concreta y pertinente al reactivo al recomendar que los gobiernos promuevan campañas para difundir dichas estrategias (proyección). Deficiencias: lenguaje algo redundante y una imprecisión menor en la redacción final (p. ej. 'enseñaran' debería ser 'enseñen'); la proyección podría precisarse más (qué tipo de campañas, alcance), pero cumple los dos requisitos exigidos.</t>
+          <t>La conclusión cumple ambos aspectos: sintetiza la idea principal (teletrabajo compatible con la salud si se aplican estrategias concretas: espacio, horario, ritual de cierre) y plantea una proyección concreta (los gobiernos deberían promover campañas). Deficiencias específicas: no aborda de forma explícita la preocupación central del reactivo sobre el 'hogar' como último refugio en peligro; la proyección es limitada al actor gubernamental (faltarían empleadores, políticas laborales o servicios de salud mental); contiene un error verbal ('enseñaran' → 'enseñen') y cierta formulación redundante. Recomiendo mantener la síntesis pero añadir una mención explícita a la protección del hogar como refugio y ampliar los agentes responsables en la proyección.</t>
         </is>
       </c>
       <c r="D37" s="2" t="inlineStr">
         <is>
-          <t>Los párrafos están claramente identificables y hay conectores lógicos (p. ej. “En primer lugar”, “Por otro lado”), por lo que la estructura básica es adecuada. Sin embargo, existe repetición: el párrafo 5 (conclusión) repite la tesis del párrafo 1 («es posible realizar teletrabajo de manera sana») y además reitera las tres estrategias ya desarrolladas en los párrafos 2–4 (espacio definido, horarios, ritual de cierre). Esa reiteración en un párrafo anterior califica como un caso de repetición en un párrafo, por lo que corresponde NIVEL 3 según la escala. Para alcanzar NIVEL 4 (mínima corrección): reformular el párrafo final para que aporte un subtema distinto (por ejemplo, detallar medidas de política pública concretas, prioridades de intervención gubernamental o limitaciones y ámbitos de investigación futuros) en lugar de volver a enunciar la tesis y las mismas estrategias.</t>
+          <t>Los párrafos están claramente identificables y responden al reactivo: Párrafo 1 (introducción y tesis), Párrafo 2 (espacio físico en el hogar), Párrafo 3 (respeto de horarios), Párrafo 4 (ritual de cierre y prácticas alternativas). Hay conectores lógicos entre párrafos ("En primer lugar", "Por otro lado", "Hay quienes...", "En conclusión"). Sin embargo, el Párrafo 5 (conclusión) repite de manera explícita las mismas estrategias ya desarrolladas en los párrafos 2–4 y retoma la tesis del párrafo 1; esa repetición en un solo párrafo impide otorgar la puntuación máxima según la escala. No se observan otras repeticiones entre los párrafos temáticos 2–4.</t>
         </is>
       </c>
     </row>
@@ -1040,60 +1028,60 @@
         <v>10</v>
       </c>
       <c r="B38" s="2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C38" s="2" t="n">
         <v>2</v>
       </c>
       <c r="D38" s="2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="2" t="n"/>
       <c r="B39" s="2" t="inlineStr">
         <is>
-          <t>Aunque aparecen los cuatro elementos básicos de forma superficial (qué: el sistema de enseñanza tras la pandemia; quiénes: 'la población chilena' en una mención general; dónde: Chile implícito; cuándo: 'a raíz de la pandemia' / 'en la actualidad'), la introducción es vaga y poco específica. No se identifican actores relevantes por nombre (p. ej. estudiantes, docentes, Ministerio, familias) ni se delimita con precisión el tema (no distingue entre enseñanza virtual y presencial ni el alcance del problema). Además el enunciado de tesis ('las clases presenciales son la solución') se presenta como afirmación sin contextualización ni referencia al debate planteado en el reactivo. Para alcanzar nivel 4 haría falta mayor especificidad en actores y periodo y una formulación clara y justificada del problema.</t>
+          <t>El primer párrafo identifica el tema (sistema de enseñanza tras la pandemia) y ubica el contexto espacial (población chilena) y temporal de forma general ('en la actualidad', 'a raíz de la pandemia'). Sin embargo, los elementos no son lo suficientemente específicos ni completos: 'quiénes' queda reducido a 'población chilena' sin identificar actores clave (estudiantes, docentes, Ministerio en la introducción), y 'cuándo' es vago (no precisa periodo, etapa de la pandemia ni fechas). Además el párrafo adopta una postura (las clases presenciales son la solución) en lugar de presentar el marco informativo del reactivo, por lo que la introducción no cumple con la función neutral y precisa requerida.</t>
         </is>
       </c>
       <c r="C39" s="2" t="inlineStr">
         <is>
-          <t>El cierre intenta recapitular la postura (clases presenciales como solución) pero no realiza una síntesis en palabras realmente nuevas: repite las mismas afirmaciones ya expuestas. Tampoco ofrece una proyección con implicaciones, recomendaciones, consecuencias políticas o condiciones para la reapertura; la única mención ('desafío planteado por el Ministerio de Educación') no desarrolla acciones, plazos ni consideraciones prácticas. Hay intento de cierre, pero carece de estructura analítica y prospectiva.</t>
+          <t>Hay una síntesis explícita: el texto reitera que las clases presenciales son la solución para déficit de aprendizaje y problemas de salud. No obstante, la síntesis es básicamente repetitiva (frases casi idénticas a lo ya dicho) y carece de proyección: no ofrece consecuencias, recomendaciones prácticas, condiciones para la reapertura, ni reflexión sobre riesgos o medidas futuras. Tampoco introduce matices ni evaluación de evidencia, por lo que el cierre es insuficiente para un ensayo argumentativo.</t>
         </is>
       </c>
       <c r="D39" s="2" t="inlineStr">
         <is>
-          <t>La progresión es parcial: cada párrafo aborda un subtema distinto (introducción, aprendizaje, salud nutricional/mental, riesgo de contagio, conclusión), y existen conectores («Por una parte», «Por otra parte», «Sin embargo»). Sin embargo hay repetición evidente entre párrafos: el primer y el último párrafo repiten la misma tesis; el párrafo final retoma prácticamente sin variación las conclusiones de los párrafos 2 y 3. Además algunos párrafos están pobremente desarrollados y ofrecen afirmaciones generales o datos sin discusión ni transición analítica, lo que debilita la coherencia global. Según la rúbrica, esa repetición parcial limita el nivel máximo a 3.</t>
+          <t>La estructura presenta párrafos con subtemas (introducción, aprendizaje, salud nutricional/mental, contrapunto sobre contagio, conclusión) y conectores lógicos ('Por una parte', 'Por otra parte', 'Sin embargo', 'De esta manera'). Aun así, hay redundancia: el párrafo final reproduce ideas y formulaciones ya expuestas (vuelve a afirmar la solución presencial varias veces) y no aporta información nueva ni síntesis profunda; además algunas afirmaciones carecen de enlace analítico entre evidencia y conclusión. En consecuencia, la progresión no es totalmente eficaz: un párrafo (el cierre) repite parcialmente información de los anteriores y debilita el avance argumental.</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="2" t="n"/>
       <c r="B40" s="2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C40" s="2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D40" s="2" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="2" t="n"/>
       <c r="B41" s="2" t="inlineStr">
         <is>
-          <t>La introducción contiene el 'qué' (el sistema de enseñanza implementado a raíz de la pandemia) en forma general, pero es poco específica. El 'dónde' aparece sólo de manera implícita/indirecta al mencionar "la población chilena" en la última oración (no queda explícito en las primeras dos oraciones), y el 'quiénes' no se identifican de forma concreta: no se nombran actores clave por tipo o por institución (por ejemplo: estudiantes, docentes, familias, Ministerio de Educación) sino un grupo genérico. El 'cuándo' es vago («En la actualidad») y carece de un periodo o fecha precisa relacionada con la pandemia (p. ej. desde marzo de 2020, 2020–2022, etc.). Además, la introducción no articula claramente el conflicto planteado en el reactivo (posturas pro-presencialidad vs. pro-permanencia en modalidad virtual) ni identifica a los actores relevantes del debate. Por estas deficiencias (temporal impreciso y actores poco concretos) se ubica en Nivel 3.</t>
+          <t>Qué: Sí (tema: el sistema de enseñanza implementado a raíz de la pandemia y la necesidad de presencialidad) y Dónde: Sí (se alude a la población chilena, lo que sitúa el texto en Chile). Quiénes: Insuficiente; la introducción no nombra actores concretos (p. ej. estudiantes, docentes, padres, Ministerio de Educación) sino una referencia genérica a la "población chilena". Cuándo: Vago; expresiones como "En la actualidad" y "a raíz de la pandemia" no ofrecen un periodo concreto (fechas o intervalo). Además, respecto al reactivo, la introducción adopta una postura a favor de la presencialidad sin presentar la contraparte (quienes prefieren mantener la virtualidad por salud), por lo que no responde plenamente al dilema planteado. Por estas ausencias y vaguedades se asigna 2 puntos.</t>
         </is>
       </c>
       <c r="C41" s="2" t="inlineStr">
         <is>
-          <t>El texto presenta un cierre identificable que reafirma la tesis (las clases presenciales como solución), por lo que existe un comentario conclusivo; sin embargo falla en la síntesis porque repite literalmente la idea principal en lugar de reformularla con nuevas palabras y mayor precisión. Tampoco ofrece una proyección adecuada: no plantea implicaciones concretas, consecuencias operativas ni contexto futuro (la mención vaga de un “desafío planteado” por el Ministerio es insuficiente). Responde al reactivo de forma afirmativa pero de manera superficial y reiterativa, sin el cierre prospectivo exigido.</t>
+          <t>Hay un cierre identificable que defiende claramente la reapertura presencial (por tanto responde al reactivo), pero presenta deficiencias: no hay una síntesis reformulada de la idea principal (repite literalmente la tesis ya expresada en la introducción y en el cuerpo) y carece de proyección significativa (solo menciona de forma vaga el “desafío” del Ministerio sin plantear implicaciones, consecuencias o reflexiones futuras). En suma, es un cierre tipo comentario, no una conclusión sintética y proyectiva.</t>
         </is>
       </c>
       <c r="D41" s="2" t="inlineStr">
         <is>
-          <t>Los párrafos son claramente identificables y hay conectores lógicos (</t>
+          <t>El texto tiene cinco párrafos claramente identificables y presenta conectores lógicos ("Por una parte", "Por otra parte", "Sin embargo", "De esta manera"). Sin embargo, hay repetición evidente de la idea central (“las clases presenciales son la solución”): el Párrafo 1 afirma la solución de forma categórica y la misma conclusión vuelve a aparecer en el Párrafo 2 (aunque con datos), en el Párrafo 4 (al refutar riesgos de contagio) y en el Párrafo 5 (conclusión redundante). Los Párrafos 2, 4 y 5 repiten información ya planteada en el Párrafo 1, por lo que al menos dos (en realidad tres) párrafos recuperan la misma idea principal en vez de desarrollar subtemas claramente distintos. Para alcanzar puntaje 3 se requieren correcciones mínimas y concretas: a) transformar el Párrafo 1 en una introducción neutral que presente el debate sin declarar la solución; b) mantener en el Párrafo 2 el foco en el déficit de aprendizaje (con la estadística) sin reiterar la conclusión; c) centrar el Párrafo 4 exclusivamente en la evidencia sobre contagio sin volver a argumentar la solución; d) convertir el Párrafo 5 en una síntesis breve que integre sin repetir literalmente que “las clases presenciales son la solución”. Así se asegurarían subtemas distintos por párrafo y se evitaría la repetición.</t>
         </is>
       </c>
     </row>
@@ -1102,10 +1090,10 @@
         <v>11</v>
       </c>
       <c r="B42" s="2" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C42" s="2" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D42" s="2" t="n">
         <v>2</v>
@@ -1115,24 +1103,24 @@
       <c r="A43" s="2" t="n"/>
       <c r="B43" s="2" t="inlineStr">
         <is>
-          <t>Tiene el 'qué' (la encíclica Fratelli Tutti y la postura del Papa) y un 'quién' claro (el Papa Francisco). Sin embargo 'cuándo' aparece solo como una frase vaga ('en el último tiempo') y 'dónde' no se especifica en absoluto (no hay contexto espacial ni institucional preciso). Además no nombra otros actores relevantes por nombre o categoría explícita en la introducción (por ejemplo: movimientos sociales, tradición filosófica católica medieval, órdenes franciscanas), lo que impide situar el tema según el REACTIVO. Corrección sugerida: incluir un marco temporal concreto, un ámbito espacial o institucional y nombrar los actores en conflicto/diálogo desde el inicio.</t>
+          <t>El texto presenta claramente el qué (la encíclica Fratelli Tutti y su contenido) y el quién (el Papa Francisco). Sin embargo, falla en el dónde y el cuándo: 'en su encíclica' es un contexto genérico (no señala un lugar o ámbito espacial concreto) y la referencia temporal ('en el último tiempo') es vaga. Por tanto solo dos elementos son identificables con claridad; se requiere indicar un marco espacial/contextual más preciso y una periodización explícita (fecha, año de la encíclica o periodo histórico) para alcanzar puntaje mayor.</t>
         </is>
       </c>
       <c r="C43" s="2" t="inlineStr">
         <is>
-          <t>Hay una reformulación de la idea principal (síntesis) en el último párrafo, pero es repetitiva y no aporta una reformulación sustancial en términos nuevos. La 'proyección' existe solo de manera genérica y retórica ('hacer un mundo mejor', 'invita a practicarla'), sin especificar consecuencias, implicaciones concretas, recomendaciones prácticas o contextos futuros. No hay un cierre analítico que indique qué implicaría aceptar la propuesta del Papa en términos políticos o sociales. Corrección sugerida: añadir proyección explícita (efectos esperables, retos, implicaciones políticas o sociales) y una síntesis en lenguaje distinto al del cuerpo del texto.</t>
+          <t>Hay un intento de cierre en el último párrafo, pero este consiste mayormente en reiteraciones del contenido anterior sin reformulación clara de la idea central ni enunciados nuevos que sinteticen en palabras distintas. La proyección es mínima y genérica ('hacer un mundo mejor para todos') sin implicaciones, consecuencias concretas ni líneas futuras de acción o reflexión. Es necesario una síntesis novedosa de la tesis y una proyección explícita (consecuencias, escenarios o recomendaciones) para mejorar la conclusión.</t>
         </is>
       </c>
       <c r="D43" s="2" t="inlineStr">
         <is>
-          <t>El texto tiene párrafos reconocibles pero presenta redundancias significativas: el primer párrafo y el último repiten la misma tesis central con escasas variantes; además el segundo y cuarto párrafos retoman ideas ya expuestas (solidaridad, condena del individualismo) sin desarrollar subtemas claramente distintos. Los conectores lógicos son limitados y las transiciones entre párrafos son débiles, de modo que no se perciben subtemas autónomos por párrafo ni una sucesión argumentativa bien organizada. También falta un tratamiento equilibrado de la posición contraria mencionada en el REACTIVO (no se presenta ni refuta con detalle el argumento de que la propuesta sanciona una forma de vida explotadora). Corrección sugerida: reestructurar para que cada párrafo trate un subtema distinto (contexto/autoridad, explicación conceptual de solidaridad, relación con la tradición medieval y crítica opuesta, consecuencias/práctica) y evitar la repetición literal de la tesis.</t>
+          <t>La estructura presenta párrafos con subtemas susceptibles de ser distintos (tesis; definición de solidaridad; papel del Papa frente a la tradición; cierre), pero el último párrafo repite parcial y enunciativamente información ya desarrollada (condena del individualismo, defensa del bien común y la solidaridad, llamado a alinear la vida personal) que solapa con el primer y segundo párrafo. Además, los conectores y transiciones son escasos, lo que reduce la coherencia. Para mejorar: evitar reiteraciones, asignar a cada párrafo un subtema verdaderamente distinto y añadir marcadores discursivos que articulen la progresión argumental.</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="2" t="n"/>
       <c r="B44" s="2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C44" s="2" t="n">
         <v>3</v>
@@ -1145,17 +1133,17 @@
       <c r="A45" s="2" t="n"/>
       <c r="B45" s="2" t="inlineStr">
         <is>
-          <t>Solo están claros el 'Qué' (tema: la encíclica Fratelli Tutti y la postura sobre justicia social, individualismo y solidaridad) y el 'Quién' (Papa Francisco, mencionado por nombre). Falta un 'Dónde' explícito (no se indica país, región o contexto espacial concreto) y el 'Cuándo' aparece solo de forma vaga ('en el último tiempo', 'actual') sin periodo, fecha o marco temporal preciso. El pasaje es pertinente al reactivo (sostiene que Francisco va más allá de la tradición), pero no cumple los cuatro elementos específicos exigidos.</t>
+          <t>La introducción presenta claramente el Qué (tema: la encíclica Fratelli Tutti y su defensa de la solidaridad frente al individualismo) y el Quiénes (el Papa Francisco) de forma específica. Sin embargo, no cumple el Dónde — no aporta ninguna ubicación geográfica o contexto espacial concreto — ni el Cuándo — sólo emplea una expresión vaga («en el último tiempo») sin periodo, fecha ni marco histórico preciso. Respecto al reactivo, el texto trata la tesis central (sintonía con reclamos sociales y su relación con la tradición), pero la ausencia de lugar y tiempo impide alcanzar la introducción completa exigida.</t>
         </is>
       </c>
       <c r="C45" s="2" t="inlineStr">
         <is>
-          <t>El texto presenta un cierre reconocible que resume la postura central (que Francisco propone una alternativa social que condena el individualismo y promueve la solidaridad), por lo que existe un comentario conclusivo. Sin embargo, falla en la SÍNTESIS exigida: predominan la repetición y la reiteración de ideas ya expuestas en lugar de una reformulación clara y novedosa de la tesis. Asimismo, la PROYECCIÓN es débil y vaga: el cierre alude a la intención del pontífice de ‘hacer un mundo mejor’, pero no plantea consecuencias concretas, implicaciones claras ni escenarios o reflexiones futuras relevantes sobre cómo se traduciría esa propuesta en cambios sociales o políticos. Por eso no alcanza el nivel 4.</t>
+          <t>La sección final cumple ambos aspectos exigidos: sintetiza la tesis central (que Francisco elabora y promueve una propuesta social cristiana que condena el individualismo y busca el desarrollo integral mediante justicia, caridad y solidaridad) en nuevas palabras y plantea una proyección: la necesidad de alinear la vida de las personas con esa propuesta para lograr un mundo mejor. Deficiencias específicas: la proyección es genérica y carece de concreción sobre mecanismos, plazos o actores concretos; no aborda con claridad la objeción contraria presentada en el reactivo; el cierre repite ideas ya expuestas y contiene problemas menores de puntuación que afectan la claridad. Pese a ello, existe un cierre distinguible que concluye y proyecta la tesis, por lo que corresponde 3 puntos.</t>
         </is>
       </c>
       <c r="D45" s="2" t="inlineStr">
         <is>
-          <t>El texto tiene párrafos claramente identificables y responde al reactivo (sitúa a Francisco entre la tradición y una propuesta activa). Sin embargo hay repetición de información en dos párrafos: el párrafo 3 y el párrafo 4 retoman y repiten la misma idea central expuesta en el párrafo 1 (que el Papa no se limita a describir la tradición, sino que elabora, promueve y practica una propuesta social que condena el individualismo). Además el párrafo 4 vuelve a reiterar el objetivo y los destinatarios de la propuesta (invitar a todos, condena del individualismo, alineamiento de la vida con el bien común), información ya presentada en los párrafos 1 y 3. Aunque existen conectores entre párrafos (p. ej. “Para conseguir esto…”, “El Papa no se queda solo…”), la progresión se ve afectada por esas repeticiones, que impiden que cada párrafo presente un subtema claramente distinto sin solapamientos. Para alcanzar Nivel 4 habría que eliminar o reubicar la reiteración del párrafo 4 (concretar allí una conclusión nueva o datos disjuntos) y matizar el párrafo 3 para que aporte un aspecto distinto y no repita el enunciado general del párrafo 1.</t>
+          <t>El texto presenta cuatro párrafos claramente identificables y contiene conectores que enlazan las ideas (p.ej. “Para conseguir esto...”, “El Papa no se queda solo...”). Los párrafos 1, 2 y 3 desarrollan subtemas distintos: (p.1) tesis general sobre la encíclica y la condena del individualismo; (p.2) la solidaridad cristiana como motor del cambio; (p.3) la relación del Papa con la tradición y su papel activo en formular una propuesta. Sin embargo, el párrafo 4 repite información ya expresada en p.1 (condena del individualismo y promoción del bien común) y en p.3 (que Francisco crea, promueve e invita a practicar una propuesta social), por lo que hay repetición de ideas en un párrafo. Para alcanzar puntaje 3 se requiere una corrección mínima: modificar el párrafo 4 para que aporte un subtema distinto (por ejemplo, consecuencias prácticas de la propuesta, audiencia concreta a la que se dirige o mecanismos de implementación) o eliminar las frases que reiteran p.1 y p.3.</t>
         </is>
       </c>
     </row>
@@ -1164,10 +1152,10 @@
         <v>12</v>
       </c>
       <c r="B46" s="2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C46" s="2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D46" s="2" t="n">
         <v>2</v>
@@ -1177,47 +1165,47 @@
       <c r="A47" s="2" t="n"/>
       <c r="B47" s="2" t="inlineStr">
         <is>
-          <t>Solo cumple el elemento 'qué' (prácticas de autocuidado frente a factores ambientales). Falta identificar 'quiénes' (no nombra especialistas, instituciones concretas ni autores), 'dónde' (no especifica el contexto espacial requerido por el reactivo: p. ej. grandes ciudades o entornos urbanos) y 'cuándo' (no hay periodo temporal ni marco histórico). La apertura es genérica y no enmarca el alcance ni las fuentes del argumento exigido por el reactivo.</t>
+          <t>Solo identifica de manera general el tema (prácticas de autocuidado frente a factores ambientales), es decir el 'qué'. No aparecen explícitamente el 'quién' (no se mencionan especialistas, instituciones o autores concretos), el 'dónde' (no se alude a las grandes ciudades ni a un contexto espacial preciso del reactivo) ni el 'cuándo' (no hay periodo temporal ni marco histórico). Además el inicio usa una voz pasiva vaga ('Se ha demostrado') que oculta la fuente y reduce la especificidad. Sugerencia: incluir una frase introductoria que nombre a los especialistas o instituciones, precise el contexto urbano (p. ej. 'en las grandes ciudades') y, si procede, un marco temporal o actualidad.</t>
         </is>
       </c>
       <c r="C47" s="2" t="inlineStr">
         <is>
-          <t>Ofrece una síntesis parcial (pide información más honesta y priorizar la integridad personal frente a intereses) pero carece de proyección explícita: no indica consecuencias concretas, líneas de acción futuras ni implicaciones de política pública en relación con la afirmación del reactivo sobre la ineficacia de medidas individuales ante causas ambientales. Es cierre descriptivo pero sin proyección ni recomendaciones operativas.</t>
+          <t>Hay un intento de cierre y una proyección (criticar la promoción guiada por intereses, pedir honestidad y orientar la promoción hacia la integridad personal), pero falta una síntesis clara que reformule la idea principal en palabras nuevas: el texto no reexpresa de forma precisa y condensada que las medidas individuales ayudan pero no cambian las condiciones ambientales estructurales (tal como plantea el reactivo). La proyección es algo genérica y no articula consecuencias políticas ni recomendaciones concretas para abordar las causas del problema. Sugerencia: añadir una oración final que sintetice la tesis (beneficios individuales vs. insuficiencia para corregir causas estructurales) y una proyección concreta sobre políticas o acciones colectivas necesarias.</t>
         </is>
       </c>
       <c r="D47" s="2" t="inlineStr">
         <is>
-          <t>Hay estructura de párrafos, pero existe redundancia: el primer párrafo (afirmación general) se repite parcialmente en los párrafos 3 y 4 que describen beneficios de las prácticas y reformulan la misma idea; además la transición hacia la crítica sistémica (párrafo 5) resulta algo abrupta. Hay conectores básicos ('pero', 'desde', 'todas'), pero la información no avanza de manera netamente acumulativa ni cada párrafo aporta un subtema claramente distinto. No se responde con precisión al contexto urbano/específico planteado por el reactivo (contaminación en grandes ciudades).</t>
+          <t>La estructura en párrafos existe, pero presenta redundancias y conectores débiles. Los párrafos 3 y 4 repiten funciones y beneficios de las prácticas de autocuidado (enumeración de efectos positivos y la idea de enfoque preventivo), por lo que aportan información parcialmente redundante. Hay escasez de conectores que articulen claramente la transición desde los beneficios individuales hacia la crítica de su insuficiencia sistémica; el párrafo 2 plantea una pregunta retórica que no encamina la progresión argumental. Además, la crítica al marketing y la llamada a la honestidad vuelven a ideas ya insinuadas, sin avance temático claro. Sugerencia: condensar los párrafos que enumeran beneficios en uno solo, utilizar conectores explícitos para marcar el giro hacia la crítica sistémica y reordenar para que cada párrafo aporte un subtema distinto y progresivo.</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="2" t="n"/>
       <c r="B48" s="2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C48" s="2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D48" s="2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="2" t="n"/>
       <c r="B49" s="2" t="inlineStr">
         <is>
-          <t>Qué: Sí está presente y claro: el tema central es la eficacia limitada de las prácticas de autocuidado frente a factores ambientales nocivos. Quiénes: Insuficiente. No hay actores identificados por nombre; aparecen referencias vagas («instituciones y marcas», «la medicina», «la población») que no cumplen el requisito de actores concretos. Dónde: Ausente. No se especifica ubicación geográfica ni contexto espacial (por ejemplo, «grandes ciudades» mencionado en el reactivo no aparece en el texto). Cuándo: Ausente. No se indica periodo temporal, fecha o momento histórico. Además, la introducción no conecta explícitamente con el reactivo (no cita a los especialistas en medicina ni la contaminación del aire en ciudades).</t>
+          <t>Solo 1 elemento claramente identificable. Qué: presente en la primera oración (prácticas de autocuidado y hábitos saludables frente a factores ambientales). Quiénes: ausentes o demasiado vagos; el texto alude a 'la medicina', 'instituciones y marcas' y 'la población' pero no nombra actores concretos como 'especialistas en medicina' o instituciones específicas. Dónde: ausente; no se indica una ubicación precisa (por ejemplo 'grandes ciudades' o contexto urbano). Cuándo: ausente; no hay periodo temporal, fecha ni referencia histórica precisa. Pertinencia al reactivo: parcial: recoge la idea general de que las medidas individuales no solucionan el problema, pero no reproduce ni especifica el reclamo central del reactivo (la afirmación de especialistas sobre la protección frente a la contaminación del aire en grandes ciudades).</t>
         </is>
       </c>
       <c r="C49" s="2" t="inlineStr">
         <is>
-          <t>El cierre cumple como comentario final pero falla en la síntesis exigida: no reformula con claridad la idea principal (que el autocuidado ayuda pero no sustituye cambios estructurales frente a la contaminación) sino que ofrece una recomendación puntual sobre honestidad en la difusión. La proyección existe pero es superficial y limitada a una apelación ética (promoción honesta, integridad), sin plantear implicaciones, consecuencias o escenarios futuros concretos (políticas públicas, reformas regulatorias, impacto social). Responde parcialmente al reactivo, pero no integra ni sintetiza la tesis ni desarrolla una proyección sólida; por ello no alcanza nivel 4.</t>
+          <t>El texto presenta un cierre a modo de comentario (pide mayor honestidad en la difusión y que el autocuidado sea por integridad personal), pero no ofrece una síntesis clara que reformule en nuevas palabras la idea central (que las prácticas individuales ayudan pero no solucionan las causas estructurales de la contaminación) ni una proyección desarrollada (implicaciones políticas, sociales o escenarios futuros). Responde tangencialmente al reactivo, pero carece de reformulación de la tesis y de consecuencias o recomendaciones concretas y explícitas.</t>
         </is>
       </c>
       <c r="D49" s="2" t="inlineStr">
         <is>
-          <t>El texto presenta párrafos claramente identificables y responde al reactivo (reconoce beneficios del autocuidado y su limitación ante problemas estructurales), pero hay repetición de información en varios párrafos. Concretamente: el párrafo 4 repite y amplía lo ya expuesto en el párrafo 3 sobre los beneficios de las prácticas de autocuidado; el párrafo 5 retoma la tesis del párrafo 1 sobre la insuficiencia de las acciones individuales y añade la exigencia de cambios de política (repetición temática); el párrafo 6 vuelve a la crítica sobre intereses y la promoción, que ya aparece en el párrafo 5. Además, los conectores entre párrafos son superficiales y las transiciones resultan abruptas, lo que debilita la progresión textual. Para alcanzar un nivel 4 sería necesario que cada párrafo trate un subtema claramente distinto sin solapamientos y que las transiciones organicen lógicamente el avance del argumento.</t>
+          <t>Los párrafos son identificables y el texto responde al reactivo (reconoce que el autocuidado ayuda pero no soluciona las causas estructurales), pero hay repeticiones claras que rompen la progresión: el Párrafo 1 y el Párrafo 5 reiteran la misma tesis central (que las medidas individuales son parche y no sustituyen cambios de política), y el Párrafo 6 vuelve a la misma crítica sobre intereses y honestidad informativa; además, el Párrafo 3 (beneficios fisiológicos) y el Párrafo 4 (ventaja y popularidad de las prácticas) se traslapan al tratar los mismos efectos positivos. También faltan conectores lógicos más explícitos que marquen avance temático entre algunos párrafos (por ejemplo, entre la enumeración de prácticas y la exposición de sus efectos, o entre la constatación de beneficios y la crítica política). Corrección mínima sugerida para alcanzar 3 puntos: evitar repetir la idea de que las medidas individuales no sustituyen políticas (fusionar o eliminar uno de P1/P5/P6), reservar un párrafo exclusivamente para beneficios concretos (P3), otro para impacto social y cambio de enfoque sanitario (reformular P4 para que no repita P3), y convertir el último párrafo en una conclusión breve que conecte con políticas públicas usando conectores claros (p. ej. 'Sin embargo', 'Por tanto').</t>
         </is>
       </c>
     </row>
@@ -1226,40 +1214,40 @@
         <v>13</v>
       </c>
       <c r="B50" s="2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C50" s="2" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D50" s="2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="2" t="n"/>
       <c r="B51" s="2" t="inlineStr">
         <is>
-          <t>El texto identifica el qué (pandemia de COVID-19) y el dónde (Chile) y aporta referencias temporales (finales del semestre pasado; finales de febrero/comienzo de marzo; plebiscito en octubre), pero falla en el elemento 'quiénes' exigido: no nombra actores relevantes del reactivo (p. ej. Servel, cifras de electores, autoridades concretas) y algunos marcadores temporales son vagos ('finales del semestre pasado'). Además la introducción no sitúa explícitamente la cuestión central del reactivo (la exclusión de pacientes con PCR positivo del voto) ni contextualiza con los actores e instituciones que toman la decisión.</t>
+          <t>El texto identifica el tema central (la pandemia de COVID-19) y el lugar (China y Chile) y ofrece referencias temporales vagas («finales del semestre pasado», «finales de febrero y comienzo de marzo»). Sin embargo no nombra actores relevantes (por ejemplo: Servel, el plebiscito del 25 de octubre, autoridades concretas) y las indicaciones temporales son imprecisas. Además no conecta explícitamente la pandemia con la medida concreta descrita en el reactivo (prohibición de votar a pacientes PCR positivos), por lo que la introducción queda incompleta y poco específica.</t>
         </is>
       </c>
       <c r="C51" s="2" t="inlineStr">
         <is>
-          <t>Hay un intento de síntesis: se reitera el derecho y deber de votar y se plantea que negar el voto a contagiados es discriminatorio; sin embargo la conclusión es contradictoria al aceptar simultáneamente que la medida gubernamental está 'implementada de buena forma' sin desarrollar consecuencias. No hay proyección ni implicaciones futuras claras (no propone medidas, alternativas ni escenarios futuros), por lo que cumple la síntesis de forma tenue pero carece de un cierre prospectivo fundamentado.</t>
+          <t>Hay un intento de cierre que reitera la idea de derecho al voto y denuncia de discriminación, pero no hay una síntesis reformulada de la idea principal ni una proyección clara (implicaciones, recomendaciones o consecuencias futuras). La conclusión además es contradictoria (afirma discriminación pero también que la medida está bien implementada) y no estructura un cierre argumental.</t>
         </is>
       </c>
       <c r="D51" s="2" t="inlineStr">
         <is>
-          <t>La organización es redundante: múltiples párrafos repiten la misma idea sobre el riesgo de contagio y la imposibilidad de votar (párr. 2, 3, 4 y 5 repiten argumentos similares). No hay desarrollo de subtemas diferenciados (antecedentes, marco institucional, argumentos jurídicos, propuestas sanitarias), faltan conectores lógicos y varias ideas se repiten con variaciones léxicas. Además el texto no aborda aspectos claves del reactivo (por ejemplo la mención explícita a Servel, la restricción por PCR positivo y las cifras electorales), lo que evidencia una progresión pobre y desordenada.</t>
+          <t>El texto presenta varios párrafos que repiten las mismas ideas sobre el riesgo sanitario y la imposibilidad de votar: el segundo, tercero y cuarto párrafo redundan parcialmente. Faltan conectores lógicos que ordenen la argumentación y cada párrafo no desarrolla un subtema distinto ni aporta evidencia nueva. Además omite elementos clave del reactivo (mención explícita de Servel, la fecha del plebiscito 25 de octubre, la medida sobre pacientes PCR positivos), lo que impide una progresión temática coherente.</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="2" t="n"/>
       <c r="B52" s="2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C52" s="2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D52" s="2" t="n">
         <v>1</v>
@@ -1269,17 +1257,17 @@
       <c r="A53" s="2" t="n"/>
       <c r="B53" s="2" t="inlineStr">
         <is>
-          <t>El texto presenta 'Dónde' (Chile) y referencias temporales (llegada a finales de febrero/ principios de marzo; mención a 'octubre'), pero falla en precisión y concreción de los demás elementos exigidos. 'Qué' está disperso y no hay una oración temática clara que defina el foco: la introducción ofrece antecedentes sobre la pandemia pero no enuncia explícitamente el problema concreto (la exclusión de votantes contagiados). 'Quiénes' es vago: aparecen expresiones genéricas ('el presidente', 'muchas personas', 'adultos mayores') pero no se nombran actores clave ni grupos concretos exigidos por el reactivo (por ejemplo, el Servicio Electoral —Servel— y los electores afectados, o cifras). Además no se cita la medida específica del Servel ni la fecha exacta del plebiscito (25 de octubre). Para alcanzar NIVEL 4 se necesita añadir 1–2 oraciones iniciales muy concretas que incluyan: (1) el qué: 'el impacto de la decisión del Servicio Electoral (Servel) de impedir votar a pacientes con PCR positivo', (2) quiénes: 'Servel y los electores contagiados (indicar cifras si se dispone)', (3) dónde: 'Chile', y (4) cuándo: 'plebiscito del 25 de octubre de 2020'.</t>
+          <t>Presenta 'Dónde' (China; Chile) y 'Cuándo' (llegada feb-mar; plebiscito en octubre; Constitución de 1980). El 'Qué' (la pandemia y sus efectos sobre la votación) aparece pero de forma dispersa y poco precisa; no está formulado en 1-2 oraciones claras y no focaliza el reactivo (la medida específica del Servel: prohibición de votar a pacientes PCR+ y la discusión sobre discriminación). Falta por completo 'Quiénes' con nombres concretos o actores identificables (por ejemplo Servel, Presidente por nombre, grupos afectados concretos). Por esas deficiencias no alcanza el puntaje máximo.</t>
         </is>
       </c>
       <c r="C53" s="2" t="inlineStr">
         <is>
-          <t>El texto tiene un cierre reconocible («Ahora bien en conclusión...») que comenta sobre el derecho a voto y la supuesta discriminación de contagiados, por lo que funciona como un comentario final. No cumple una síntesis rigurosa: no reformula con claridad y en nuevas palabras la idea principal del texto, sino que repite afirmaciones dispersas sobre derechos y riesgos. Tampoco ofrece proyección: no plantea consecuencias concretas, reflexiones profundas, escenarios futuros ni propuestas relacionadas con el reactivo. Además presenta una contradicción no resuelta (denuncia discriminación pero al mismo tiempo justifica la medida por salud pública) sin analizar sus implicaciones. Por todo ello corresponde Nivel 3.</t>
+          <t>La conclusión funciona como un comentario final que retoma la idea central (derecho/deber de votar y la exclusión de contagiados) pero no realiza una síntesis clara y reformulada de la tesis: la formulación es breve, redundante y con ambigüedades (p. ej. 'todos el voto de uno puede hacer el cambio', contradicciones entre denunciar discriminación y avalar la medida). Además carece de proyección: no plantea consecuencias, recomendaciones ni reflexiones a futuro sobre la exclusión de pacientes PCR positivos ni su impacto jurídico o social. Responde de forma parcial al reactivo (menciona la exclusión), pero omite un análisis prospectivo necesario.</t>
         </is>
       </c>
       <c r="D53" s="2" t="inlineStr">
         <is>
-          <t>El texto tiene párrafos identificables, pero la progresión es deficiente porque varios párrafos repiten esencialmente las mismas ideas y carecen de enlaces lógicos claros. Párrafo 1 (origen y ‘nueva realidad’) y párrafo 2 (convocatoria y aplazamiento del plebiscito) presentan subtemas distintos; sin embargo, los párrafos 3, 4, 5 y 6 reiteran de forma redundante la misma preocupación central (riesgo de contagio al votar, personas que no votarán por miedo o por estar enfermas, asintomáticos y la tensión entre derecho al voto y protección de la vida). Es decir: 3 párrafos o más vuelven a la misma información ya expuesta (riesgo de contagio y privación del voto a contagiados), además de concluir con una contradicción no resuelta. Tampoco hay conectores interparrafales que organicen avance argumental (transición, contraste o ejemplificación) y el texto no atiende con precisión el reactivo: no menciona la decisión del Servel ni el criterio de PCR positivo ni el planteamiento jurídico sobre igualdad/discriminación requerido. Por estas razones la repetición generalizada y la ausencia de conectores justifican el NIVEL 1.</t>
+          <t>El texto presenta párrafos claramente identificables (6), pero al menos dos párrafos repiten información previa: el párrafo 4 repite ideas ya expresadas en los párrafos 2 (imposibilidad de votar de contagiados) y 3 (riesgo de contagio en votaciones), y el párrafo 6 vuelve a reiterar tanto la posible discriminación de los contagiados como el argumento sanitario de riesgo ya dicho en los párrafos 3 y 4. Además, el párrafo 5 sobre transmisión asintomática solapa parcialmente el argumento de riesgo del párrafo 3 en lugar de aportar un subtema nuevo y específico. Hay escasos o nulos conectores lógicos entre párrafos, por lo que la progresión temática es débil. En cuanto a pertinencia al reactivo, el texto no menciona elementos claves del enunciado (por ejemplo, la decisión del Servel y la exclusión de pacientes con PCR positivo) ni analiza con precisión la acusación de discriminación legal, por lo que no responde plenamente al reactivo. Para llegar a puntaje 3 se requieren correcciones mínimas: reorganizar los párrafos para que cada uno trate un subtema distinto (1: origen y contexto de la pandemia; 2: calendario del plebiscito y la decisión concreta del Servel/PCR; 3: riesgos sanitarios de la votación incluyendo transmisión asintomática —fusionar párrafos 3 y 5—; 4: impacto sobre la participación (adultos mayores, hospitalizados); 5: análisis jurídico y ético sobre si la medida constituye discriminación; 6: conclusión clara), eliminar enunciados repetidos, y añadir conectores transicionales breves entre párrafos.</t>
         </is>
       </c>
     </row>
@@ -1288,10 +1276,10 @@
         <v>14</v>
       </c>
       <c r="B54" s="2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C54" s="2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D54" s="2" t="n">
         <v>1</v>
@@ -1301,47 +1289,47 @@
       <c r="A55" s="2" t="n"/>
       <c r="B55" s="2" t="inlineStr">
         <is>
-          <t>El texto menciona claramente el qué (la rebaja de la indemnización por el Caso Soquimich) y nombra a un actor clave (Julio Ponce Lerou), y ubica el asunto en 'la historia reciente de Chile' (dónde). Sin embargo, el cuándo es vago ('historia reciente' no es una fecha o periodo concreto) y faltan otros actores claramente relevantes citados en el reactivo (la Corte Suprema, los fondos de pensiones, críticos y defensores). Además hay errores formales ('indeminzación') y la introducción termina abruptamente con una pregunta incompleta, lo que reduce su especificidad y coherencia.</t>
+          <t>Presente el Qué (rebaja de la indemnización) y el Quién (Julio Ponce Lerou) y menciona el Dónde (Chile). Falta el Cuándo: no se indica periodo, fecha o contexto temporal concreto ('historia reciente' es vago). Además la oración es imprecisa respecto al hecho puntual (no menciona la decisión de la Corte Suprema, montos ni votación) y contiene errores formales ('indeminzación'), lo que debilita la especificidad exigida para una introducción completa.</t>
         </is>
       </c>
       <c r="C55" s="2" t="inlineStr">
         <is>
-          <t>No existe conclusión ni cierre: el texto termina en una pregunta incompleta y no ofrece síntesis de la idea principal ni proyección sobre implicaciones o consecuencias. No reformula el argumento ni indica reflexiones futuras, por lo que no cumple ninguna de las funciones requeridas.</t>
+          <t>No hay síntesis ni proyección. El texto termina en una pregunta inaugural y está truncado; no ofrece reformulación de la idea principal ni indica implicaciones, consecuencias o una reflexión futura. No existe cierre identificable.</t>
         </is>
       </c>
       <c r="D55" s="2" t="inlineStr">
         <is>
-          <t>Es un fragmento unitario y truncado que no desarrolla subtemas ni presenta párrafos diferenciados. No hay conectores ni continuidad argumentativa, tampoco responde a los elementos del reactivo (montos, votación de la Corte Suprema, afectación a fondos de pensiones, posiciones de críticos/defensores). La estructura es inexistente y el texto no progresa.</t>
+          <t>El texto consiste en una oración afirmativa seguida de una pregunta retórica y no desarrolla subtemas ni párrafos diferenciados. No hay avance ni estructura: falta desarrollo argumental, transición entre ideas y párrafos que aporten nueva información (está truncado). No se responde al reactivo (faltan detalles clave: montos, votación, postura de críticos/defensores).</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="2" t="n"/>
       <c r="B56" s="2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C56" s="2" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D56" s="2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="2" t="n"/>
       <c r="B57" s="2" t="inlineStr">
         <is>
-          <t>La introducción contiene el Qué (la rebaja de la indemnización por el Caso Soquimich) y los Quiénes (Julio Ponce Lerou y la Corte Suprema) y el Dónde (Chile). Sin embargo carece del Cuándo: sólo alude a la "historia reciente de Chile", expresión vaga que no aporta una fecha o periodo preciso. Además omite actores clave mencionados en el reactivo (por ejemplo, los fondos de pensiones / personas que cotizan) y datos concretos del fallo (montos y votación) que son relevantes para la legitimidad planteada. El texto también termina de forma abrupta, presenta un error tipográfico («indeminzación») y signos de interrogación irregulares. Para alcanzar Nivel 4 sería necesario añadir un periodo temporal específico (fecha o año) y, brevemente, incorporar los otros actores o datos clave señalados en el reactivo.</t>
+          <t>Qué: presente (rebaja de la indemnización en el Caso Soquimich). Quiénes: presente (menciona a Julio Ponce Lerou y la Corte Suprema). Dónde: presente (Chile). Cuándo: ausente o demasiado vago («historia reciente de Chile» no es un periodo temporal preciso). Además, la introducción no responde con precisión al reactivo: omite datos clave (monto sancionado y monto rebajado, votación 3-2 de la Corte, y el efecto sobre los fondos de pensiones). También presenta errores formales e incompletitud (palabra mal escrita “indeminzación”, mayúscula innecesaria en “¿Qué”, interrogación inconclusa), lo que reduce su pertinencia y claridad.</t>
         </is>
       </c>
       <c r="C57" s="2" t="inlineStr">
         <is>
-          <t>Hay una tentativa de síntesis al afirmar que la rebaja forma parte de una serie de irregularidades en la historia reciente de Chile, pero la formulación es vaga y en buena medida repetitiva respecto al reactivo. Además presenta errores y falta de cierre (p. ej., 'indeminzación' mal escrito y una interrogación final incompleta). No cumple la proyección: no plantea consecuencias, implicaciones ni reflexión futura sobre la legitimidad del fallo ni su impacto en los fondos de pensiones. La conclusión está amalgamada y no cierra claramente el texto.</t>
+          <t>No hay una conclusión: el texto es un fragmento interrogativo e incompleto que no reformula la idea principal ni plantea proyecciones. Faltan ambos criterios: síntesis (no resume en nuevas palabras la tesis sobre la rebaja de la multa y su alcance) y proyección (no indica implicaciones legales, sociales o para el sistema de pensiones). Además presenta deficiencias formales que impiden cierre académico (palabra mal escrita 'indeminzación', puntuación incoherente). No responde al reactivo sobre la legitimidad del fallo ni sus consecuencias para los cotizantes.</t>
         </is>
       </c>
       <c r="D57" s="2" t="inlineStr">
         <is>
-          <t>El texto consta de un único párrafo muy breve e incompleto, por lo que no hay progresión textual entre párrafos: no se identifican subtemas distintos, ni se desarrollan argumentos sucesivos. El contenido se limita a afirmar que la rebaja es parte de irregularidades y a formular una pregunta retórica sin elaborar; no hay conectores que orienten un avance temático ni separación en párrafos con ideas principales distintas. Además presenta errores formales (p. ej. “indeminzación”) y la pregunta final queda truncada, de modo que no responde ni desarrolla los elementos del reactivo (críticas, defensa del sistema de pensiones, impacto en cotizantes). Según la escala, ante la ausencia de estructura pluripárrafo y la falta de progresión se justifica asignar el nivel más bajo.</t>
+          <t>El texto consta de un solo párrafo incompleto y no desarrolla subtemas distintos ni una secuencia argumental. Al haber únicamente un párrafo no se cumple la exigencia de progresión entre párrafos (falta de conectores y transición), y además la oración final queda truncada (pregunta sin respuesta), por lo que el reactivo no se aborda ni se articula. Deficiencias específicas: 1) ausencia de párrafos con subtemas diferenciados; 2) falta total de conectores o transiciones entre párrafos (imposible evaluarlos por existir solo uno); 3) el contenido no responde ni desarrolla la cuestión planteada sobre la legitimidad del fallo de la Corte Suprema. Por estas razones, y aplicando criterio estricto, el puntaje es 0.</t>
         </is>
       </c>
     </row>
@@ -1350,60 +1338,60 @@
         <v>15</v>
       </c>
       <c r="B58" s="2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C58" s="2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D58" s="2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="2" t="n"/>
       <c r="B59" s="2" t="inlineStr">
         <is>
-          <t>El texto identifica el qué (confinamiento, teletrabajo y efectos sobre la salud mental) y el cuándo (la pandemia / COVID-19) y alude al dónde de forma general ('en gran parte del mundo', 'lugares cerrados'), pero falla en presentar actores específicos con claridad: solo aparecen referencias vagas ('la población', 'trabajadores', 'familias', 'muchas empresas') sin nombrar agentes relevantes ni diferenciar sujetos clave. Además la 'introducción' no es concisa ni claramente delimitada (se extiende enunciando consecuencias), por lo que no cumple la expectativa de 1–2 oraciones precisas que sitúen explícitamente el tema en relación con el REACTIVO (p. ej. la amenaza al hogar como refugio). Sugerencia: redactar 1–2 frases iniciales que contengan explícitamente Qué, Quiénes (grupos/actores concretos), Dónde (ámbito espacial preciso) y Cuándo.</t>
+          <t>El texto presenta el 'qué' (confinamiento/teletrabajo y efectos en salud mental) y el 'cuándo' (pandemia/COVID‑19) y ofrece referencias espaciales generales ('lugares cerrados', 'gran parte del mundo'), pero falla en identificar con precisión 'quiénes' (no nombra actores concretos: empleadores, trabajadores por sectores, autoridades sanitarias, familias, etc.). Además la presentación es difusa y extensa, no formula una tesis clara vinculada al reactivo (la Salud del hogar como refugio en riesgo). Para mejorar: incluir en las primeras oraciones el tema en una frase concisa, nombrar los actores afectados y precisar el ámbito espacial/temporal, y formular una tesis que responda explícitamente al reactivo.</t>
         </is>
       </c>
       <c r="C59" s="2" t="inlineStr">
         <is>
-          <t>El texto carece de una conclusión estructurada. El párrafo final repite ideas ya expuestas (estrés laboral, incapacidad de desconectar, aumento de síntomas ansiosos) pero no ofrece una síntesis reformulada de la tesis central ni una proyección (implicaciones, recomendaciones, consecuencias futuras o líneas de investigación). Hay un intento difuso de cierre temático, pero sin reescribir la idea principal en nuevas palabras ni indicar implicaciones concretas respecto al peligro que enfrenta el hogar como refugio, exigencias normativas o consecuencias para políticas de salud mental. Sugerencia: añadir un párrafo final que sintetice la tesis y presente al menos una proyección o recomendación relacionada con el REACTIVO.</t>
+          <t>Hay un párrafo final que intenta cerrar, pero no cumple con la síntesis ni con la proyección exigidas: repite afirmaciones sobre estrés y pérdida de calidad de vida sin reformular la idea central en términos nuevos y sin ofrecer implicaciones, consecuencias concretas, recomendaciones o líneas de investigación futuras. Tampoco liga el cierre con la idea central del reactivo (la 'salud' del hogar como último refugio). Se requiere una oración de síntesis clara y al menos una proposición de proyección (políticas, riesgos futuros o medidas) para subir el puntaje.</t>
         </is>
       </c>
       <c r="D59" s="2" t="inlineStr">
         <is>
-          <t>La organización presenta redundancias y falta de conectores claros. Varios párrafos repiten información: el primero y el tercero reiteran el aumento de trastornos ansiosos/depresivos y la presión sobre servicios de salud; el segundo y el cuarto vuelven sobre la alteración de horarios, la imposibilidad de desconectar y la pérdida de soporte social. No hay una progresión evidente por subtemas (p. ej. contexto → consecuencias laborales → impacto en la vida familiar → propuestas), y faltan conectores lógicos que articulen transiciones. Además hay oraciones extensas y errores que dificultan la coherencia interna. Sugerencia: reorganizar para que cada párrafo trate un subtema distinto y emplear conectores que marquen relaciones (causa-efecto, contraste, ejemplificación).</t>
+          <t>El texto tiene varios párrafos pero presenta redundancia importante: el aumento de trastornos ansiosos/depresivos y la afectación de la salud mental se repiten en los párrafos 1, 2 y 4 sin aportar información nueva; el párrafo 3 añade el dato del aumento de consultas y ansiolíticos pero sin conexión lógica ni datos precisos. Faltan conectores que articulen causa, consecuencia y ejemplos; las ideas están enunciadas en oraciones largas y con errores que dificultan la separación temática. Para corregir: asignar a cada párrafo un subtema distinto (p. ej. 1=definición y alcance, 2=impacto laboral y temporización, 3=impacto familiar/espacial, 4=datos y propuestas), evitar repeticiones y añadir transiciones explícitas.</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="2" t="n"/>
       <c r="B60" s="2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C60" s="2" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D60" s="2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="2" t="n"/>
       <c r="B61" s="2" t="inlineStr">
         <is>
-          <t>La introducción presenta parcialmente el elemento 'Qué' (habla de confinamiento, teletrabajo y aumento de ansiedad/depresión) y el 'Cuándo' (la pandemia/COVID-19), pero falla en los otros dos elementos exigidos. 'Quiénes' aparece solo con términos genéricos («la población», «trabajadores», «familias», «miles de personas») y no identifica actores concretos por nombre o categoría precisa (por ejemplo: trabajadores de oficina, padres con hijos en edad escolar, personal sanitario, empleadores). 'Dónde' es vago: usa expresiones generales («en muchas partes del mundo», «en el hogar», «lugares cerrados») en lugar de una ubicación geográfica o contexto espacial específico (país, ciudad, ámbito urbano/rural o contexto doméstico claramente delimitado). Además, el 'Qué' aunque presente está difuso y no se enuncia en 1–2 oraciones claras que articulen la tesis central requerida por el reactivo (la posible afectación de la salud del hogar como refugio frente al teletrabajo). Para alcanzar NIVEL 4 se requiere: 1) condensar el tema en 1–2 oraciones claras que enuncien la tesis central vinculada al reactivo; 2) nombrar actores concretos relevantes; y 3) precisar una ubicación espacial concreta (país, ciudad o contexto claramente delimitado).</t>
+          <t>Se otorga 1 punto. El texto contiene el 'qué' (impacto del teletrabajo/confinamiento en la salud mental) y el 'cuándo' (la pandemia/COVID-19), pero incumple los otros requisitos. 'Quiénes' aparecen solo como referencias genéricas ('la población', 'trabajadores', 'familias', 'muchas empresas') y no como actores concretos por nombre; 'Dónde' es vago ('en muchas partes del mundo', 'lugares cerrados') y no ofrece una ubicación geográfica o contexto espacial específico. Además el 'qué' no está formulado de manera clara y concisa en 1-2 oraciones, sino disperso en varios párrafos, por lo que la introducción carece de la especificidad exigida por el reactivo.</t>
         </is>
       </c>
       <c r="C61" s="2" t="inlineStr">
         <is>
-          <t>El texto presenta un cierre reconocible a modo de comentario que resume consecuencias (síntesis parcial: el teletrabajo impide desconectarse y ha afectado la calidad de vida), por lo que sí existe una conclusión breve. Sin embargo, la proyección es débil: sólo enumera efectos inmediatos (aumento de ansiedad) y no plantea implicaciones futuras, recomendaciones ni reflexiona sobre la idea específica del reactivo (el hogar como último refugio). Además, la síntesis es general y poco elaborada, sin cerrar con una reflexión prospectiva; por ello corresponde nivel 3.</t>
+          <t>La estructura no presenta un cierre claro; el párrafo final funciona como continuación del desarrollo más que como conclusión. Déficits específicos: falta una síntesis explícita que reformule con claridad la idea principal (no se resume que el hogar como refugio está en peligro por el teletrabajo) y no hay proyección (no se plantean implicaciones futuras, recomendaciones o reflexiones prospectivas). Además, la conclusión no responde plenamente al reactivo porque no aborda de forma puntual la noción del hogar como último refugio ni sus consecuencias futuras.</t>
         </is>
       </c>
       <c r="D61" s="2" t="inlineStr">
         <is>
-          <t>El texto presenta cuatro párrafos claramente identificables, pero en dos de ellos se repite información previa: el párrafo 3 repite la idea general del párrafo 1 (aumento de problemas de ansiedad y demanda de atención psiquiátrica/medicación como efecto del confinamiento) y el párrafo 4 reitera nuevamente la misma consecuencia (empeoramiento de la calidad de vida y aumento de signos ansiosos), solapándose con P1 y P3. El párrafo 2 aporta un subtema distinto (alteración de la dinámica laboral y pérdida de límites), por lo que es novedoso. Además hay conectores escasos y poco coherentes entre párrafos (solo aparece “Por otro lado”; en general faltan transiciones que articulen causa/efecto y jerarquicen las ideas). Finalmente, el texto no aborda con claridad el aspecto central del reactivo sobre la “salud del hogar” como refugio amenazado: menciona efectos sobre la salud mental y la convivencia, pero no desarrolla ni evidencia cómo se pone en peligro la noción de hogar refugio. Estas deficiencias justifican el NIVEL 2.</t>
+          <t>Se identifican cuatro párrafos claramente diferenciables. Sin embargo, hay repetición de la misma idea central (deterioro de la salud mental: aumento de ansiedad/ansiedad y uso de fármacos) en tres párrafos (párrafos 2, 3 y 4 repiten la consecuencia ya enunciada en el párrafo 1), por lo que la información no progresa con subtemas verdaderamente distintos. Hay conectores entre párrafos 1→2 (“A pesar de...”) y 2→3 (“Por otro lado”), pero el párrafo 4 carece de transición clara y añade contenido repetido en vez de un subtema nuevo. Además, la respuesta al reactivo es sólo parcial: el texto discute impactos del teletrabajo y del confinamiento sobre la salud mental, pero no aborda de forma específica y desarrollada la idea propuesta en el reactivo sobre la “salud del lugar llamado hogar” como último refugio amenazado. Deficiencias concretas: repetición temática en párrafos 2, 3 y 4; ausencia de un subtema exclusivo en el último párrafo; transiciones débiles e insuficiente focalización en la noción del hogar como espacio protegido.</t>
         </is>
       </c>
     </row>
@@ -1415,57 +1403,57 @@
         <v>2</v>
       </c>
       <c r="C62" s="2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D62" s="2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="2" t="n"/>
       <c r="B63" s="2" t="inlineStr">
         <is>
-          <t>La introducción solo cumple parcialmente: define de manera vaga el tema central (cierre de colegios y clases virtuales) y menciona actores genéricos ('el gobierno', 'los colegios'), pero falla en especificidad. No indica un lugar concreto (dónde) ni un periodo temporal claro (cuándo: 'actual' es impreciso). Además no presenta explícitamente las posiciones enfrentadas que plantea el reactivo (los 'algunos' a favor de mantener la virtualidad y los 'otros' que piden reapertura), por lo que no configura una introducción completa ni contextualizada. Sugerencia: incluir fecha o periodo, ámbito geográfico y nombrar con precisión los actores relevantes o los grupos señalados en el reactivo y exponer brevemente las dos posturas en disputa.</t>
+          <t>El texto presenta el tema central (cierre de colegios y clases virtuales) y menciona actores genéricos (“el gobierno”, “colegios”), además alude al momento como “actual contexto sanitario”. Sin embargo, faltan especificidad espacial (no indica país/ámbito concreto) y la referencia temporal es vaga. Tampoco introduce con claridad las posiciones contrapuestas del reactivo (p. ej. quienes priorizan la salud mental de los niños), por lo que la introducción no sitúa plenamente el conflicto planteado. Sugerencia: explicitar lugar y periodo, nombrar con precisión los actores relevantes y enunciar brevemente ambas posturas del reactivo.</t>
         </is>
       </c>
       <c r="C63" s="2" t="inlineStr">
         <is>
-          <t>La conclusión ofrece una reformulación de la idea central (síntesis) al reiterar que la virtualidad protege la salud y mejora accesibilidad, pero no cumple la función de proyección: no indica consecuencias futuras, recomendaciones políticas, implicaciones educativas ni reflexiones sobre cómo implementar o evaluar esa postura. Además es básicamente repetitiva y carece de sugerencias o pasos siguientes. Sugerencia: añadir proyección concreta (impacto esperado, medidas necesarias, seguimiento o criterios para evaluar el retorno a la presencialidad) y reformular la síntesis en términos no redundantes.</t>
+          <t>Hay una síntesis del argumento principal (las clases virtuales protegen la salud y favorecen accesibilidad), pero falta proyección: no se indican implicaciones futuras, recomendaciones de política, consecuencias a mediano/largo plazo ni reflexión sobre la otra cara del reactivo (salud mental/emocional). La conclusión vuelve a enumerar puntos previos sin reformularlos críticamente ni plantear pasos siguientes. Sugerencia: añadir una proyección explícita (p. ej. medidas para mitigar efectos en salud mental, criterios para volver a la presencialidad o evaluación de métodos pedagógicos).</t>
         </is>
       </c>
       <c r="D63" s="2" t="inlineStr">
         <is>
-          <t>La progresión presenta párrafos con subtemas distintos (contexto/posición, salud, accesibilidad, crítica y respuesta, conclusión), pero hay repetición parcial entre el primer párrafo y el segundo (ambos insisten en el argumento de protección sanitaria y cierre de colegios), lo que reduce la cohesión. Faltan conectores lógicos claros entre párrafos y algunas transiciones son abruptas; el cuarto párrafo introduce el contraargumento pero lo desarrolla de manera insuficiente y sin enlace sólido con el anterior. Sugerencia: eliminar redundancias (fusionar o diferenciar con más precisión el primer y segundo párrafo), usar conectores explícitos para guiar el avance argumental y desarrollar mejor la oposición antes de refutarla.</t>
+          <t>La estructura tiene párrafos con subtemas diferenciables (introducción/tesis, salud y riesgo de contagio, igualdad por transporte, objeción sobre aprendizaje, conclusión), y hay conectores; sin embargo, hay redundancia: el primer y segundo párrafo repiten la misma idea central sobre protección de la salud con formulaciones muy próximas. Además la objeción sobre salud mental señalada en el reactivo queda poco desarrollada, por lo que no hay equilibrio en la progresión argumental. Sugerencia: eliminar repeticiones, consolidar la idea de salud en un solo párrafo y desarrollar con mayor profundidad la objeción contraria para fortalecer la coherencia argumental.</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="2" t="n"/>
       <c r="B64" s="2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C64" s="2" t="n">
         <v>3</v>
       </c>
       <c r="D64" s="2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="2" t="n"/>
       <c r="B65" s="2" t="inlineStr">
         <is>
-          <t>Solo el elemento 'Qué' aparece claramente: plantea el cierre de colegios y la defensa de la continuidad de las clases virtuales (tesis). Los demás elementos están ausentes o vagos: 'Quiénes' se menciona de forma genérica ('el gobierno', 'colegios', 'escolares') pero no identifica actores concretos por nombre; 'Dónde' no aparece (no hay país, región o contexto espacial específico); 'Cuándo' es impreciso ('actual contexto sanitario') y no se refiere explícita y datadamente a la pandemia (p. ej. periodo o fecha). Además, la introducción no sitúa la controversia del reactivo (las voces que piden reapertura por salud mental) con actores concretos, lo que reduce su pertinencia. Para alcanzar NIVEL 4 sería necesario incorporar: ubicación geográfica precisa, periodo temporal concreto (por ejemplo, 'desde marzo de 2020'), y actores nombrados (p. ej. 'Ministerio de Educación', 'padres de familia', 'estudiantes') de forma explícita.</t>
+          <t>Presenta claramente el 'qué' (la transformación a clases virtuales y la tesis de que los colegios no deben volver a la presencialidad). Sin embargo, 'quiénes' está tratado de forma vaga: aparecen referentes genéricos ('el gobierno', 'los colegios', 'los escolares') sin identificar actores concretos ni instituciones específicas. 'Dónde' está ausente: no se indica país, región ni contexto espacial preciso. 'Cuándo' es impreciso: se alude al 'actual contexto sanitario' pero no hay periodo o fechas claras dentro de la introducción. La postura es pertinente al reactivo, pero la falta de especificidad en quiénes, dónde y cuándo impide un puntaje mayor.</t>
         </is>
       </c>
       <c r="C65" s="2" t="inlineStr">
         <is>
-          <t>Existe un cierre identificable que vuelve a afirmar la tesis y los argumentos centrales (seguridad sanitaria, protección de la salud, igualdad de acceso), por lo que hay síntesis aunque resulta repetitiva y poco reformulada. Sin embargo, falta proyección: no plantea implicaciones, consecuencias, recomendaciones ni perspectivas futuras, ni aborda el contraargumento relevante sobre la salud mental y emocional de los estudiantes. En conjunto, es un cierre tipo comentario que no cumple la proyección exigida por el reactivo.</t>
+          <t>La conclusión sintetiza la tesis principal (defensa de la continuidad de las clases virtuales) en nuevas palabras y presenta consecuencias relevantes (aprendizaje seguro, protección de la salud, mayor igualdad de acceso), por lo que cumple síntesis y proyección básicas. Deficiencias específicas: repite argumentos ya expuestos sin profundizar ni ofrecer una proyección temporal o recomendaciones concretas; la proyección es descriptiva y limitada (no plantea consecuencias futuras, acciones políticas ni reflexiones prospectivas); además presenta problemas de redacción y cohesión que reducen su fuerza argumentativa.</t>
         </is>
       </c>
       <c r="D65" s="2" t="inlineStr">
         <is>
-          <t>El texto presenta párrafos claramente identificables y responde al reactivo (defiende mantener la enseñanza virtual). Sin embargo hay al menos dos párrafos que repiten información previa: el párrafo 2 repite la idea central del párrafo 1 (las clases virtuales resguardan la salud y permiten la continuidad educativa) y el párrafo final (conclusión) vuelve a enunciar los mismos beneficios (aprendizaje seguro, resguardo de la salud y igualdad de acceso). Los conectores entre párrafos existen (p. ej. "En este escenario", "Al realizar...", "En el mismo contexto", "No obstante", "En conclusión"), por lo que la coherencia transicional está atendida; la falla es la repetición de contenido en dos párrafos distintos, lo que encaja con NIVEL 2. Sugerencia mínima para alcanzar NIVEL 4: eliminar o reformular el párrafo 2 para que aporte un subtópico distinto (por ejemplo, detallar sólo mecanismos de contagio y evidencia empírica sin reiterar la tesis) y convertir la conclusión en una síntesis breve o una recomendación concreta que no reproduzca frases ni argumentos ya expuestos.</t>
+          <t>Se otorga 1 punto. Los párrafos son claramente identificables y existen conectores entre ellos, pero hay repetición de ideas en dos párrafos: el párrafo 2 repite la idea central del párrafo 1 (protección de la salud mediante clases virtuales) y el párrafo 5 (conclusión) vuelve a reiterar ideas ya expuestas sobre salud e igualdad. Además, aunque el texto defiende la continuidad de la virtualidad, no aborda de forma suficiente la preocupación por la salud mental/emocional planteada en el reactivo, por lo que la pertinencia está incompleta.</t>
         </is>
       </c>
     </row>
@@ -1474,10 +1462,10 @@
         <v>17</v>
       </c>
       <c r="B66" s="2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C66" s="2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D66" s="2" t="n">
         <v>2</v>
@@ -1487,17 +1475,17 @@
       <c r="A67" s="2" t="n"/>
       <c r="B67" s="2" t="inlineStr">
         <is>
-          <t>La introducción identifica claramente el tema (contaminación del aire y actividad física) y el lugar general ('las grandes ciudades'), pero falla en dos elementos: 'quiénes' relevantes no están bien especificados (menciona 'las grandes empresas' y 'niños' pero no a los 'especialistas' que plantea el reactivo) y 'cuándo' es vago ('en el último tiempo'). Además no aclara la postura respecto al enunciado del reactivo (la posición de los especialistas sobre los efectos limitados de las medidas individuales). Sugerencia: nombrar explícitamente a los especialistas como actores relevantes y precisar un marco temporal o periodo concreto.</t>
+          <t>El párrafo inicial identifica el tema (contaminación del aire en las grandes ciudades) y menciona actores generales ("las grandes empresas", "niños", "educación escolar"), pero falla en la indicación temporal específica: "En el último tiempo" es vago. Además no menciona a los actores relevantes del REACTIVO (por ejemplo, "especialistas en medicina") ni sitúa con precisión el contexto histórico o periodo. Para ser completa requiere una fecha/periodo concreto y una identificación más explícita de los actores expertales referidos en el enunciado.</t>
         </is>
       </c>
       <c r="C67" s="2" t="inlineStr">
         <is>
-          <t>Hay una proyección explícita (se propone que el gobierno lance campañas o leyes) y una reformulación del tema, pero la síntesis es meramente repetitiva y no reescribe la idea principal en términos nuevos ni reconoce la limitación central del reactivo (que las medidas individuales no cambian las condiciones ambientales causantes). Además la conclusión contradice el reactivo al sostener que el ejercicio 'combatirá' el problema ambiental en lugar de plantear medidas sistémicas. Sugerencia: en la conclusión sintetizar con palabras nuevas y proyectar implicaciones reales (p. ej. políticas públicas y medidas estructurales) admitiendo los límites del autocuidado.</t>
+          <t>Hay proyección explícita (propuesta de campaña o ley gubernamental para fomentar el deporte), pero la síntesis de la idea principal es tenue y esencialmente repetitiva: no reformula la tesis en palabras nuevas ni reconoce la limitación central del REACTIVO (que las medidas individuales no atacan las causas ambientales). La conclusión además generaliza al afirmar que la actividad física "combatirá" el problema, contradiciendo sin evidencias la advertencia de los especialistas.</t>
         </is>
       </c>
       <c r="D67" s="2" t="inlineStr">
         <is>
-          <t>La organización por párrafos existe, pero hay redundancia: el párrafo 2 (beneficios del ejercicio y frecuencia recomendada) y el párrafo 3 (déficit en las escuelas e importancia de incentivar a los niños) repiten la misma idea central sobre la necesidad de fomentar deporte en niños; el párrafo 4 repite y además desestima sin fundamento la postura contraria de los especialistas. Faltan conectores y transiciones que integren el contraargumento con la tesis; la secuencia resulta repetitiva y no desarrolla subtemas claramente diferenciados. Sugerencia: condensar las ideas repetidas, usar conectores para articular evidencia, contraargumento y reconciliación con el reactivo (reconocer limitaciones individuales y proponer medidas estructurales).</t>
+          <t>El texto está dividido en párrafos y usa conectores básicos, pero presenta repetición parcial: los párrafos 2 y 3 reiteran la misma idea central (beneficios de la actividad física e importancia de fomentarla en la escuela) sin aportar subtemas claramente distintos; el párrafo 5 repite la recomendación final. El párrafo 4 introduce la objeción de los expertos pero la refuta sin argumento ni evidencia, rompiendo la coherencia argumental con el REACTIVO. Se requieren subtemas diferenciados (evidencia de beneficios, límites frente a la contaminación, políticas públicas efectivas) y mejor integración de la objeción experta.</t>
         </is>
       </c>
     </row>
@@ -1507,7 +1495,7 @@
         <v>2</v>
       </c>
       <c r="C68" s="2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D68" s="2" t="n">
         <v>1</v>
@@ -1517,17 +1505,17 @@
       <c r="A69" s="2" t="n"/>
       <c r="B69" s="2" t="inlineStr">
         <is>
-          <t>Solo el “qué” aparece con claridad: la contaminación del aire como problema. Los “quiénes” son vagos: menciona “las grandes empresas” y “los niños” pero no actores concretos ni los especialistas en medicina que plantea el reactivo. El “dónde” es genérico (“las grandes ciudades”) y no especifica contexto geográfico preciso. El “cuándo” falta por completo (no hay periodo temporal ni fecha). Además la introducción no refleja la postura clave del reactivo sobre la posición de los especialistas (que, pese a recomendar ejercicio, señalan que las acciones individuales no cambian las condiciones causantes), sino que afirma categóricamente que el deporte resolverá el problema, lo que reduce su pertinencia respecto al reactivo.</t>
+          <t>La introducción contiene el Qué (contaminación del aire y la propuesta de fomentar actividad física) y un Dónde genérico («las grandes ciudades»), y menciona actores generales (Quiénes: «las grandes empresas», «los niños»), pero varios elementos son vagos o imprecisos. El Qué no está claramente formulado en 1–2 oraciones centrándose en un solo tema (mezcla problema ambiental y propuesta educativa). El Quiénes son grupos indefinidos; no hay actores concretos por nombre (p. ej., gobierno, ministerio, ciudades específicas, empresas concretas). El Dónde es demasiado general («grandes ciudades») y el Cuándo es vago («En el último tiempo»). Además, la introducción no refleja con fidelidad el matiz del reactivo: el reactivo señala que el autocuidado ayuda pero no modifica las condiciones que causan la contaminación; la introducción afirma que fomentar deporte «combatirá» el problema sin reconocer esa limitación. Por tanto, hay 2–3 elementos presentes pero expresados de forma general, por eso corresponde 2 puntos.</t>
         </is>
       </c>
       <c r="C69" s="2" t="inlineStr">
         <is>
-          <t>La conclusión funciona como un cierre a modo de comentario: repite la idea principal (contaminación y la importancia del deporte) pero la síntesis es débil y poco reformulada, limitándose a reiterar lo ya dicho. Sí presenta una proyección (propone campañas o leyes gubernamentales), pero es vaga (“alguna campaña o ley”) y no aborda correctamente el reactivo: no reconoce la limitación señalada por especialistas de que las medidas individuales no modifican las causas ambientales y, además, contradice implícitamente esa advertencia al afirmar que el ejercicio ‘combate’ el problema. En conjunto, hay cierre comentativo pero falta una síntesis clara y una proyección precisa y coherente con el reactivo.</t>
+          <t>El cierre cumple como comentario: contiene una síntesis parcial (menciona la contaminación y recomienda actividad física) y una proyección (propone campaña o ley). No alcanza 3 puntos porque la síntesis es reiterativa y poco reformulada, y—sobre todo—la conclusión no responde al reactivo: omite la precisión de los especialistas de que las medidas individuales no modifican las condiciones que generan la contaminación y, en cambio, afirma que el ejercicio 'combate' el problema. Sugerencia breve: reformular reconociendo que la actividad física mejora la resistencia individual pero no sustituye medidas estructurales, y mantener la propuesta de políticas públicas dirigidas a reducir la contaminación.</t>
         </is>
       </c>
       <c r="D69" s="2" t="inlineStr">
         <is>
-          <t>Aunque los párrafos son identificables, el texto presenta repetición sistemática de las mismas ideas y no desarrolla subtemas realmente distintos. Párrafo 1 introduce el problema y propone fomentar la actividad física en la educación; Párrafo 2 vuelve a afirmar el beneficio del ejercicio (repetición del argumento de Párrafo 1, aunque con detalle de frecuencia); Párrafo 3 repite la misma propuesta educativa (idéntica idea central que Párrafo 1); Párrafo 4 retoma otra vez la afirmación de que el ejercicio protege frente a la contaminación y además contradice sin fundamento la postura contraria, por lo que reutiliza la misma noción ya expuesta; Párrafo 5 es una conclusión que resume y repite las propuestas de Párrafos 1 y 3 (nueva repetición). Sí hay conectores parciales ('Por una parte', 'Por otra parte', 'En conclusión'), pero no bastan para crear subtemas diferenciados ni evitar la redundancia. Además el texto no atiende plenamente el reactivo: omite desarrollar la idea clave de que las medidas individuales no modifican las condiciones que generan la contaminación (la solución estructural), limitándose a repetir la promoción del deporte. Por estas deficiencias (repetición en múltiples párrafos y omisión de la segunda parte del reactivo) corresponde Nivel 1.</t>
+          <t>El texto tiene párrafos claramente identificables pero presenta repeticiones en más de dos párrafos y falla en responder con precisión el reactivo. Repeticiones detectadas: Párrafo 1 y Párrafo 3 (ambos proponen cambiar la educación para fomentar la actividad física); Párrafo 1 y Párrafo 5 (la idea de promover deporte desde la infancia y la responsabilidad gubernamental se repite); Párrafo 2 y Párrafo 4 (ambos afirman que el ejercicio protege los pulmones ante la contaminación, P4 además rechaza la conclusión del reactivo). Conectores existen (“Por una parte”, “Por otra parte”, “Sin embargo”), pero no evitan la reiteración de ideas. Además, el texto no atiende correctamente el reactivo: los especialistas señalan que el autocuidado mejora la resistencia individual pero no modifica las condiciones que provocan la contaminación; el texto, en cambio, niega esa limitación y sugiere que el ejercicio por sí solo mitiga el problema ambiental. Para alcanzar puntaje 3 sería necesario asignar subtemas distintos a cada párrafo (por ejemplo: 1) problema y causas sistémicas; 2) evidencia sobre beneficios del ejercicio; 3) límites de las medidas individuales según expertos; 4) propuestas educativas y gubernamentales complementarias; 5) conclusión) y eliminar las repeticiones señaladas.</t>
         </is>
       </c>
     </row>
@@ -1542,54 +1530,54 @@
         <v>1</v>
       </c>
       <c r="D70" s="2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="2" t="n"/>
       <c r="B71" s="2" t="inlineStr">
         <is>
-          <t>El texto presenta el 'qué' (la pandemia del COVID-19) y apunta a un 'dónde' específico (Chile), pero carece de 'quiénes' concretos (no identifica actores por nombre: autoridades, comunidades afectadas o expertos) y no indica 'cuándo' (no sitúa el periodo, p. ej. segunda ola, fechas o periodo histórico). Además la introducción es extensa y difusa: mezcla constatación y tesis sin ofrecer una apertura concisa ni conectar explícitamente con el reactivo (no aborda la segunda ola en Europa, los confinamientos sectorizados ni las acusaciones de discriminación señaladas en el enunciado).</t>
+          <t>El texto identifica claramente el qué (la pandemia del COVID-19 y sus efectos) y menciona un lugar específico (Chile), y alude a los sujetos afectados ('las personas', 'habitantes del mundo'), pero falla en la dimensión temporal: no precisa un periodo histórico o fechas relevantes (p. ej. 2020-2021, 'segunda ola'), por lo que el cuándo es vago. Además, los 'quiénes' son generales y no se nombran actores concretos (autoridades, grupos sociales específicos) solicitados por el reactivo (que habla de la segunda ola en Europa y decisiones de autoridades como la presidenta de la Comunidad de Madrid). Sugerencia: añadir un marcador temporal explícito y precisar los actores relevantes para conectar con el reactivo.</t>
         </is>
       </c>
       <c r="C71" s="2" t="inlineStr">
         <is>
-          <t>No hay conclusión identificable: el texto termina abrupto y truncado (‘q’ final) sin síntesis de la idea principal ni reformulación en otras palabras, y sin proyección (no plantea implicaciones, recomendaciones claras o escenarios futuros). Tampoco responde al reactivo en términos de cierre: no evalúa consecuencias específicas de las medidas ni reflexiona sobre la discriminación o la gestión en Europa.</t>
+          <t>Hay un intento de cierre: se reitera que el COVID-19 es un desafío para actualizar programas y normativas y se alude a la 'dignidad' y acceso a alimentos y condiciones laborales; sin embargo no hay una síntesis clara en palabras nuevas ni una proyección desarrollada y el texto termina abruptamente e incompleto ('q'), lo que impide considerar que exista una conclusión estructurada. Además no se vinculan consecuencias concretas ni se relaciona la proyección con el problema planteado en el reactivo (segunda ola, confinamientos discriminatorios). Sugerencia: redactar una oración final que reformule la tesis y exponga implicaciones políticas concretas y verificables.</t>
         </is>
       </c>
       <c r="D71" s="2" t="inlineStr">
         <is>
-          <t>El texto tiene dos párrafos que no desarrollan subtemas claramente diferenciados: ambos reiteran la necesidad de políticas públicas y la relación entre pandemia y calidad de vida, de modo que hay repetición parcial de ideas. Faltan conectores lógicos y transiciones precisas entre enunciados y párrafos; hay preguntas retóricas que no se responden ni articulan con evidencia. Además, la estructura termina de forma abrupta y no aborda elementos claves del reactivo (segunda ola europea, confinamientos por barrios, discriminación y caso de Madrid), por lo que la progresión temática no conduce a una argumentación completa.</t>
+          <t>El texto tiene separación en dos párrafos, pero no mantienen progresión totalmente nueva: el primer párrafo plantea la tesis sobre la pandemia y la necesidad de políticas públicas en Chile; el segundo repite la idea de la afectación social y la necesidad de actualizar políticas (calidad de vida, dignidad, acceso a alimentos, condiciones laborales), reconduciendo el mismo eje sin aportar subtemas claramente diferenciados. Además faltan conectores lógicos precisos y hay problemas de cohesión y frases incompletas que dificultan la transición (y el cierre incompleto). Importante: el desarrollo no responde al reactivo específico (segunda ola en Europa, confinamientos sectorizados y discriminación), por lo que la progresión temática no cumple la exigencia de abordar el caso propuesto. Sugerencia: reestructurar párrafos para que cada uno trate un subtema distinto (impacto sanitario, impacto laboral, respuesta política, ejemplo del caso europeo) y usar conectores explícitos.</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="2" t="n"/>
       <c r="B72" s="2" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C72" s="2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D72" s="2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="2" t="n"/>
       <c r="B73" s="2" t="inlineStr">
         <is>
-          <t>Presenta 3 elementos pero en forma vaga y no responde al reactivo. Qué: hay un tema central (impacto de la pandemia y necesidad de políticas) pero está disperso y no definido en 1–2 oraciones claras y específicas. Quiénes: aparecen grupos generales (“las personas en Chile”, “muchos autores”, “políticas públicas”) pero no hay actores concretos por nombre (gobierno, comunidades afectadas, grupos sociales específicos, expertos citados), por lo que es impreciso. Dónde: sí indica ubicación (Chile). Cuándo: ausente; no existe un periodo temporal preciso (p. ej. segunda ola, años, fechas). Además, el texto no es pertinente al REACTIVO, que plantea la segunda ola en Europa y casos concretos como la Comunidad de Madrid; la introducción se centra en Chile, por lo que no responde al contexto exigido.</t>
+          <t>De los cuatro elementos exigidos solo aparecen claramente el 'Qué' y el 'Dónde'. Qué: la pandemia del COVID-19 y la tesis sobre la necesidad de políticas públicas para mitigar consecuencias laborales, psicológicas y sociales (presente y relativamente específico). Dónde: se menciona explícitamente Chile. Faltan/son vagos: 'Quiénes' — no hay actores concretos nombrados (solo referencias generales: “las personas”, “muchos autores”, “políticas públicas”) cuando el reactivo exige actores específicos (por ejemplo autoridades, comunidades afectadas, migrantes, presidenta de la Comunidad de Madrid); 'Cuándo' — no se indica periodo temporal (no aparece la “segunda ola”, fechas ni marco histórico preciso). Además la introducción no responde al reactivo: el reactivo trata la segunda ola en Europa, confinamientos sectorizados y acusaciones concretas en la Comunidad de Madrid, mientras que el texto se centra de forma general en Chile, por lo que carece de pertinencia. Por estas deficiencias (solo 2 elementos identificables y falta de correspondencia con el reactivo) corresponde 1 punto.</t>
         </is>
       </c>
       <c r="C73" s="2" t="inlineStr">
         <is>
-          <t>La sección final no presenta una síntesis clara: no reformula de forma concisa la idea principal del texto en nuevas palabras, sino que repite en tono general la necesidad de políticas públicas. Existe una proyección tentativa (actualizar programas y normativas orientadas a la dignidad, acceso a alimentos y condiciones laborales), pero es superficial, desordenada y además el cierre está truncado, por lo que la proyección no se desarrolla ni concreta consecuencias futuras. Tampoco se vincula explícitamente y con pertinencia al reactivo (segunda ola europea, cuarentenas sectorizadas y discriminación), por lo que la estructura no es clara y sólo permite inferir una conclusión mezclada con el cuerpo del texto.</t>
+          <t>La pieza carece de un cierre claro y está incluso interrumpida (oración final incompleta). Si bien hay enunciados que insinúan una proyección (la necesidad de actualizar políticas públicas centradas en la dignidad, acceso a alimentos y condiciones laborales), no existe una síntesis nítida que reformule la idea principal en nuevas palabras ni un cierre estructurado. Además la proyección es vaga y no responde al reactivo específico (no aborda las cuarentenas sectorizadas, la discriminación o el contexto europeo señalado). En conjunto, la conclusión es difusa y sólo puede inferirse de manera fragmentaria.</t>
         </is>
       </c>
       <c r="D73" s="2" t="inlineStr">
         <is>
-          <t>Se asigna NIVEL 3 porque el texto presenta párrafos claramente identificables (dos), existe un conector lógico entre ellos («Conforme al objetivo anterior...») pero en un párrafo se repite información de otro: el segundo párrafo retoma y reitera la necesidad de políticas públicas y la mejora de la calidad de vida ya planteadas en el primer párrafo en lugar de desarrollar un subtema claramente distinto. Deficiencias específicas: (1) repetición temática entre párrafo 1 y párrafo 2 (políticas públicas y calidad de vida aparecen en ambos); (2) el segundo párrafo debía desarrollar un subtema distinto (por ejemplo: evidencia sobre socialización virtual, efectos psicosociales concretos, o propuestas políticas específicas) pero vuelve a exponer la tesis general; (3) el texto termina abruptamente y con errores que afectan la claridad; (4) pertinencia al REACTIVO: el texto no responde adecuadamente al enunciado dado (segunda ola en Europa, confinamientos por sectores y denuncias de discriminación) ya que se centra en Chile y en generalidades sobre políticas y socialización, sin abordar las medidas discriminatorias ni el contexto europeo solicitado.</t>
+          <t>El texto presenta dos párrafos claramente identificables. El primer párrafo expone la tesis sobre la pandemia como hito y la necesidad de políticas públicas en Chile frente a consecuencias laborales, psicológicas y sociales y a la desigualdad de acceso. El segundo párrafo aporta la idea de la condición gregaria humana y la pregunta sobre la socialización virtual, pero repite la exigencia de actualización de políticas públicas y la preocupación por la dignidad/calidad de vida ya formuladas en el primer párrafo (repetición de ideas en un párrafo). Sí existe un conector inicial (“Conforme al objetivo anterior”), pero la progresión carece de especificidad y cierre (oración final incompleta) y, además, el texto no responde al reactivo: no trata la segunda ola en Europa, los confinamientos por sectores ni la dimensión discriminatoria señalada en el enunciado. Por tanto, según la escala, corresponde 2 puntos.</t>
         </is>
       </c>
     </row>
@@ -1598,60 +1586,60 @@
         <v>19</v>
       </c>
       <c r="B74" s="2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C74" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D74" s="2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="2" t="n"/>
       <c r="B75" s="2" t="inlineStr">
         <is>
-          <t>El texto contiene un enunciado temático (qué: la pandemia de covid-19) y especifica el cuándo (año 2020), y alude a actores colectivos ('la mayoría de los países y estados del mundo') y un ámbito espacial ('del mundo'), pero esos elementos son generales y no específicos. No identifica actores por nombre ni contextos concretos, y es una sola oración que empieza abruptamente, por lo que no constituye una introducción completa. Además, no responde al reactivo: no menciona las imágenes de Venecia, los delfines, la incapacidad humana ante el ecosistema ni el modelo productivo global, temas centrales del enunciado.</t>
+          <t>El texto presenta el 'qué' (la pandemia del covid-19) y el 'cuándo' (año 2020), pero falla en especificidad de 'quiénes' y 'dónde'. 'La mayoría de los países y estados del mundo' es un actor y un lugar excesivamente general; no se mencionan actores concretos (por ejemplo: ciudadanos, personal sanitario, gobiernos, Venecia) ni un contexto espacial preciso solicitado por el reactivo (p. ej. Venecia, Italia, o canales urbanos). Además no refiere las imágenes o las posturas del reactivo (delfines/recuperación ecológica vs. imposición del modelo productivo). Sugerencia: incluir actores concretos y precisar el lugar (p. ej. Venecia) y fechas más específicas para alcanzar una introducción completa.</t>
         </is>
       </c>
       <c r="C75" s="2" t="inlineStr">
         <is>
-          <t>No existe una conclusión ni cierre: el enunciado es una afirmación única y no realiza síntesis ni reformulación de ideas en palabras nuevas, ni plantea proyección, implicaciones o reflexiones futuras. Tampoco cierra ni vincula su contenido con los puntos del reactivo (Venecia, ecosistema, modelo productivo), por lo que no cumple ninguna de las funciones requeridas.</t>
+          <t>El enunciado funciona como un intento mínimo de cierre (afirma que la pandemia será recordada por pérdidas humanas y económicas) pero carece de síntesis reformulada y, sobre todo, de proyección: no ofrece implicaciones, consecuencias ni reflexión futura sobre el tema ni dialoga con las perspectivas del reactivo (recuperación ecológica vs. modelo productivo). Es una oración final aislada sin estructura de cierre. Sugerencia: reelaborar la idea principal con otras palabras y añadir una proyección (p. ej. lecciones para políticas ambientales o económicas).</t>
         </is>
       </c>
       <c r="D75" s="2" t="inlineStr">
         <is>
-          <t>El texto es una única oración sin división en párrafos ni desarrollo de subtemas; por tanto no hay progresión textual, no se introducen ideas nuevas en párrafos sucesivos ni conectores lógicos. Tampoco responde al reactivo: no hay tratamiento ni contrastación de las posiciones sobre las imágenes de Venecia, la relación humano-ecosistema o el modelo productivo, lo que evidencia ausencia de desarrollo argumental.</t>
+          <t>El texto es una sola oración sin separación en párrafos, por lo que no cumple los requisitos de progresión: no hay desarrollo de subtemas, no hay conectores lógicos y no puede apreciarse aporte distinto por párrafo. Además no responde al reactivo en cuanto a contrastar las imágenes de Venecia y las dos posturas planteadas. Sugerencia: estructurar el texto en párrafos separados (contexto/ejemplo de Venecia; interpretación ecológica; interpretación del modelo productivo; conclusión) y usar conectores para evitar redundancias.</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="2" t="n"/>
       <c r="B76" s="2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C76" s="2" t="n">
         <v>2</v>
       </c>
       <c r="D76" s="2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="2" t="n"/>
       <c r="B77" s="2" t="inlineStr">
         <is>
-          <t>Solo aparecen 2 de los 4 elementos exigidos: 'Qué' (la pandemia del covid-19 y sus pérdidas humanas y económicas) y 'Cuándo' (año 2020). Faltan o son demasiado vagas las otras dos exigencias: 'Quiénes' no identifica actores concretos (se limita a la frase genérica «la mayoría de los países y estados del mundo» en lugar de nombrar grupos/actores específicos relevantes al reactivo, p. ej. residentes, gobiernos o comunidades de Venecia), y 'Dónde' es impreciso ('del mundo' no proporciona un contexto espacial específico; el reactivo enfatiza las aguas y canales de Venecia, que no se mencionan). Además, el texto no responde de manera pertinente al reactivo central sobre las imágenes de los canales de Venecia, los delfines y la discusión sobre la relación humano-ecosistema y el modelo productivo global.</t>
+          <t>La introducción contiene un Qué claro (la pandemia de COVID-19) y un Cuándo específico (año 2020). Sin embargo, falla en Quiénes y Dónde: "la mayoría de los países y estados del mundo" es vago y no nombra actores concretos; "del mundo" no proporciona una ubicación espacial específica (el reactivo pide, por ejemplo, referencias a Venecia y actores como delfines/ciudadanos). Además, no responde de forma pertinente al reactivo, que centra la discusión en imágenes de los canales de Venecia, debates sobre delfines y la relación humano-ecosistema/modelo productivo; ninguno de esos elementos aparece en el texto.</t>
         </is>
       </c>
       <c r="C77" s="2" t="inlineStr">
         <is>
-          <t>El enunciado final funciona como cierre tenue pero insuficiente: se limita a una afirmación general sobre pérdidas humanas y económicas (no ofrece una reformulación clara y sustancial de la idea principal del texto, por tanto falta síntesis). Tampoco plantea implicaciones, consecuencias ni proyecciones futuras relevantes sobre la tensión ecosistema/actividad humana ni sobre el modelo productivo global expuesto en el reactivo (falta proyección). En consecuencia, existe una conclusión implícita pero poco desarrollada y que no responde adecuadamente al reactivo.</t>
+          <t>El enunciado constituye un cierre a modo de comentario general sobre pérdidas humanas y económicas, por lo que encaja con el nivel 2. Sin embargo presenta deficiencias específicas: no ofrece una síntesis reformulada de las ideas centrales del reactivo (no menciona la discusión sobre Venecia, la percepción humana del ecosistema ni el modelo productivo global) y carece totalmente de proyección (implicaciones, consecuencias o reflexiones futuras). Además, es una oración final simple (que explícitamente no alcanza puntaje 3) y contiene un error ortográfico ('mayoria' → 'mayoría'). Por estas razones se otorgan 2 puntos.</t>
         </is>
       </c>
       <c r="D77" s="2" t="inlineStr">
         <is>
-          <t>El texto consiste en una sola oración/párrafo y por tanto no hay progresión entre párrafos: no se segmentan subtemas distintos, no existen conectores lógicos interparrafales y no puede valorarse continuidad temática. Además no responde al reactivo: no aborda las imágenes de Venecia, la idea de la incapacidad humana para integrarse al ecosistema ni la crítica al modelo productivo global. Deficiencias específicas: 1) ausencia de múltiples párrafos con subtemas diferenciados; 2) ausencia de conectores entre párrafos; 3) falta de pertinencia frente al reactivo.</t>
+          <t>El texto consiste en una única oración sin desarrollo ni estructura de párrafos diferenciados; por tanto no hay progresión textual. No existen párrafos con subtemas distintos ni conectores entre párrafos, y el contenido no responde al reactivo: no menciona las imágenes de Venecia, la incapacidad humana para integrarse al ecosistema ni el modelo productivo que explota a seres humanos y naturaleza. Deficiencias específicas: 1) ausencia de varios párrafos con subtemas claramente distintos; 2) ausencia de conectores que vinculen ideas; 3) falta de pertinencia frente al reactivo (tema central omitido).</t>
         </is>
       </c>
     </row>
@@ -1660,40 +1648,40 @@
         <v>20</v>
       </c>
       <c r="B78" s="2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C78" s="2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D78" s="2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="2" t="n"/>
       <c r="B79" s="2" t="inlineStr">
         <is>
-          <t>Solo cumple parcialmente el elemento 'qué' (identifica la pandemia de COVID-19) y ofrece un rasgo temporal vago ('actualmente'). Falla en especificar 'quiénes' (los actores se nombran de forma genérica: 'distintas organizaciones sanitarias' sin identificación) y 'dónde' (dice 'todos los países' en la primera frase; la referencia pertinente del reactivo es la 'segunda ola en Europa', que no aparece en la introducción). Los elementos espacial y de actores son imprecisos y el marco temporal es general; por tanto la introducción no enmarca adecuadamente el reactivo.</t>
+          <t>El texto inicia con el tema (qué: covid-19 y cuarentenas) pero no cumple los cuatro elementos exigidos. 'Quiénes' aparece de forma vaga como 'distintas organizaciones sanitarias' sin identificar actores concretos (gobiernos, autoridades locales, comunidades afectadas). 'Dónde' no se especifica: no se menciona Europa ni ningún contexto espacial concreto pese a que el reactivo exige la segunda ola europea. 'Cuándo' se limita a 'actualmente' y 'con el pasar de los meses', expresiones generales que no precisan periodo (segunda ola, meses concretos). En suma hay sólo uno o dos elementos identificables y demasiado generales; falta especificidad y conexión explícita con el reactivo.</t>
         </is>
       </c>
       <c r="C79" s="2" t="inlineStr">
         <is>
-          <t>La conclusión contiene una reformulación general (síntesis débil) al llamar a ver el COVID-19 de forma panorámica y menciona la tarea de las organizaciones sanitarias, pero carece de proyección explícita: no plantea consecuencias concretas, medidas futuras ni implicaciones políticas claras en relación con la segunda ola en Europa o las críticas por cuarentenas sectorizadas que exige el reactivo. Hay síntesis parcial pero ausencia de una proyección bien fundada.</t>
+          <t>La conclusión realiza una síntesis superficial (reformular la idea de que el covid no es solo sanitario y que hay que maximizar bienestar social) y plantea una breve orientación (las organizaciones deben maximizar bienestar), pero falla en proyección sólida: no detalla implicaciones políticas, consecuencias prácticas, medidas futuras ni evalúa el problema de la discriminación señalado en el reactivo. La proyección es vaga y normativa sin concreción (qué deben hacer, cómo, impacto esperado). Por ello hay síntesis pero la proyección es débil.</t>
         </is>
       </c>
       <c r="D79" s="2" t="inlineStr">
         <is>
-          <t>Hay redundancia clara: varios párrafos repiten las mismas ideas sobre el impacto económico/psicológico y sobre la relación entre pobreza y riesgo de contagio (párrafos 2, 3, 4 y 5 contienen solapamientos). Faltan conectores lógicos fuertes entre secciones y la delimitación de subtemas no es nítida (p.ej. separar análisis epidemiológico, criterios de cuarentena, y consecuencias socioeconómicas). Además el texto no responde con detalle al reactivo: apenas menciona la 'segunda ola en Europa' y no aborda las protestas, cuarentenas por sectores ni la acusación discriminatoria señalada en el enunciado.</t>
+          <t>La estructura muestra redundancia y escasos conectores lógicos. Dos o más párrafos repiten ideas: el párrafo 2 y el 5 reiteran la tensión teletrabajo/economía y la responsabilidad de permitir teletrabajo; el párrafo 3 y el 4 repiten que los más pobres son los más afectados y justifican restricciones por riesgo, sin aportar evidencia nueva ni matices. Faltan transiciones claras y cada párrafo no desarrolla consistentemente un subtema distinto. Además el texto no responde con precisión al reactivo: no aborda las protestas, la decisión de confinar por sectores ni la acusación discriminatoria (por ejemplo el caso de Madrid), y en cambio justifica el aislamiento de barrios pobres, lo que contradice el enfoque crítico requerido. Se requiere reorganización para evitar repeticiones y alinear contenido con el reactivo.</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="2" t="n"/>
       <c r="B80" s="2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C80" s="2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D80" s="2" t="n">
         <v>1</v>
@@ -1703,17 +1691,17 @@
       <c r="A81" s="2" t="n"/>
       <c r="B81" s="2" t="inlineStr">
         <is>
-          <t>Presenta el qué (la pandemia y las cuarentenas) y alude al dónde y cuándo al mencionar 'en Europa' y la 'segunda ola', pero lo hace de forma general. Falta el elemento 'quiénes' en forma concreta: no se nombran actores, instituciones o personas específicas (por ejemplo, autoridades sanitarias, gobiernos o la presidenta de la Comunidad de Madrid citada en el reactivo). Además, el cuándo es impreciso (no hay fechas ni periodo claramente definido) y el qué está planteado de manera amplia en lugar de centrar la tesis en 1–2 oraciones específicas relacionadas con el reactivo. Por eso corresponde NIVEL 3: falta especificidad y ausencia de actores nombrados explícitamente.</t>
+          <t>La introducción presenta el qué (la pandemia y la ‘segunda ola’) y el dónde (Europa), pero falla en la especificidad exigida. El cuándo aparece de forma vaga («actualmente», «luego de algunos meses», «segunda ola») sin un periodo temporal preciso. El quiénes está tratado de manera genérica ("personas más pobres", "organizaciones sanitarias", "expertos") y no nombra actores concretos ni instituciones relevantes del reactivo (por ejemplo, autoridades regionales o la comunidad afectada mencionada). Además no responde con precisión al enfoque del reactivo sobre confinamientos por sectores y acusaciones públicas concretas (p. ej. la referencia a la Comunidad de Madrid y su presidenta), por lo que faltan elementos específicos y pertinencia puntual.</t>
         </is>
       </c>
       <c r="C81" s="2" t="inlineStr">
         <is>
-          <t>La conclusión constituye un cierre a modo de comentario general (nivel 3): sí plantea una idea global (ver el COVID‑19 de forma panorámica y la tarea de las organizaciones sanitarias) pero no realiza una síntesis clara y reformulada de la tesis central del texto (p. ej., la crítica a los confinamientos sectorizados, la discriminación sobre barrios pobres, y las recomendaciones concretas sobre teletrabajo y responsabilidad gubernamental no se reelaboran). Tampoco ofrece una proyección concreta: faltan implicaciones, consecuencias, recomendaciones de política o escenarios futuros vinculados al reactivo (segunda ola en Europa, críticas de expertos y ejemplos como Madrid). Además, la conclusión es genérica y no responde de forma específica al problema planteado en el reactivo, por lo que no alcanza el nivel 4.</t>
+          <t>La conclusión existe y ofrece un comentario general (ver el llamado a considerar efectos más allá de lo sanitario y la necesidad de que las organizaciones sanitarias velen por el bienestar mental), por lo que no es ausencia total. Sin embargo falla en la síntesis exigida: no reformula con claridad los elementos centrales del texto y del reactivo (la segunda ola en Europa, las cuarentenas sectorizadas y su impacto discriminatorio sobre los más pobres). También adolece de proyección concreta: aporta una reflexión genérica pero no plantea implicaciones, consecuencias ni recomendaciones futuras específicas respecto al problema señalado. En suma, cierre comentado pero insuficiente para 3 puntos por su escasa pertinencia y concreción.</t>
         </is>
       </c>
       <c r="D81" s="2" t="inlineStr">
         <is>
-          <t>Aunque el texto tiene párrafos identificables y conectores (“Con el pasar...”, “Luego de...”, “Por otro lado”, “Además”, “Para concluir”), la progresión textual es deficiente porque múltiples párrafos repiten esencialmente la misma idea central (impacto socioeconómico y quién debe salir a trabajar). Específicamente: los párrafos 3, 4, 5 y 6 reiteran que los pobres son los más afectados y discuten, con variaciones, la misma propuesta de priorizar quién sale a trabajar; el párrafo 7 vuelve a resumir las mismas conclusiones. Además, el texto no responde plenamente al reactivo: omite la dimensión explícita de discriminación señalada por expertos (p. ej. acusaciones públicas como las de la Comunidad de Madrid sobre inmigrantes) y no distingue con claridad subtemas distintos (gestión de la segunda ola; criterio técnico para cuarentenas; evidencia sobre riesgo por transporte público; políticas de teletrabajo; efectos sobre salud mental). Por tanto hay más de dos párrafos que repiten información previa, lo que obliga a calificar con el nivel más bajo según la escala.</t>
+          <t>Hay párrafos claramente identificables y existen conectores entre ellos ('En este contexto', 'Con el pasar de los meses', 'Luego', 'Por otro lado', 'Además', 'Para concluir'). Sin embargo, hay repetición de ideas en varios párrafos: los párrafos 3, 4 y 5 repiten esencialmente la misma premisa sobre que las personas pobres son las más afectadas y su menor capacidad de teletrabajo; además, los párrafos 2 y 6 reiteran la dimensión económica/psicológica de la pandemia y la necesidad de permitir salir a trabajar. Por tanto no se cumple la condición de que cada párrafo tenga un subtema claramente distinto sin repetir ideas previas. Además, el texto sólo responde parcialmente al reactivo: menciona la segunda ola y la afectación de barrios pobres y críticas de expertos, pero no desarrolla la acusación discriminatoria concreta (ej. el caso de la presidenta de la comunidad de Madrid ni la dimensión explícita de medidas discriminatorias), ni describe las protestas por confinamientos sectorizados. Según la escala estricta indicada, la presencia de repetición en más de un par de párrafos obliga a asignar 1 punto.</t>
         </is>
       </c>
     </row>

</xml_diff>